<commit_message>
Add rest of feedback from wiki to SWEBOK review template
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/215cb02a53dcd42a/Mac/Research/Papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:1_{FB66D7C2-B0BB-4DB0-8057-DD9834CA6B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAEE0A9-B22F-41A2-90C2-0524F69FFC1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663CC136-25DF-459E-A583-D17E027687FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="202">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -251,9 +251,6 @@
   <si>
     <t>Reviewer's name</t>
     <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Samuel Crawford</t>
   </si>
   <si>
     <t>McMaster University</t>
@@ -579,6 +576,269 @@
   </si>
   <si>
     <t>Para. 13</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"…whether a component’s interface provides the correct…" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> "…whether the components’ interfaces provide the correct…"</t>
+    </r>
+  </si>
+  <si>
+    <t>Rewrite to avoid singular-plural mismatch</t>
+  </si>
+  <si>
+    <t>2.2.10. Interface and Application Program Interface (API) Testing</t>
+  </si>
+  <si>
+    <t>"Boundary value analysis" and "all combinations testing" throughout the document</t>
+  </si>
+  <si>
+    <t>"Fuzz testing" is the more common term used for what is called "fuzzy testing"; for example, ISO/IEC/IEEE 29119-1:2022 only uses the former</t>
+  </si>
+  <si>
+    <t>Should "Boundary-Value Analysis" and "All-Combinations Testing" have hyphens or no? They don't in ISO/IEC/IEEE 29119-4:2021, for example (see 3.3 and 3.12, respectively)</t>
+  </si>
+  <si>
+    <t>"Fuzz testing" throughout the document</t>
+  </si>
+  <si>
+    <t>More detail defining/describing evidence-based testing</t>
+  </si>
+  <si>
+    <t>Evidence-based testing isn't really defined/described, just how it applies to software engineering as a whole. What questions would be relevant? What kinds of evidence would be useful? It seems more like a "workflow" for designing other kinds of tests rather than an actual type of testing.</t>
+  </si>
+  <si>
+    <t>3.1.10. Evidence-Based</t>
+  </si>
+  <si>
+    <t>p. 5-12</t>
+  </si>
+  <si>
+    <t>p. 5-13</t>
+  </si>
+  <si>
+    <t>3.2.1. Control Flow Testing</t>
+  </si>
+  <si>
+    <t>"Control flow testing" is not defined in general</t>
+  </si>
+  <si>
+    <t>A general (but explicit) definition of "control flow testing" should be added</t>
+  </si>
+  <si>
+    <t>A explicit term and definition of control flow testing for blocks of statements should be added</t>
+  </si>
+  <si>
+    <t>A explicit term and definition of control flow testing for specific combinations of statements should be added</t>
+  </si>
+  <si>
+    <t>Control flow testing for blocks of statements is not given a name or explicitly defined</t>
+  </si>
+  <si>
+    <t>Control flow testing for specific combinations of statements is not given a name or explicitly defined</t>
+  </si>
+  <si>
+    <t>3.2.2. Data Flow Testing</t>
+  </si>
+  <si>
+    <t>"Data flow testing" is not defined in general</t>
+  </si>
+  <si>
+    <t>A general (but explicit) definition of "data flow testing" should be added</t>
+  </si>
+  <si>
+    <t>"All-definitions testing" is not explicitly defined</t>
+  </si>
+  <si>
+    <t>A explicit definition of "all-definitions testing" should be added</t>
+  </si>
+  <si>
+    <t>"All-uses testing" is not explicitly defined</t>
+  </si>
+  <si>
+    <t>A explicit definition of "all-uses testing" should be added</t>
+  </si>
+  <si>
+    <t>"All-C-uses testing" is not explicitly defined</t>
+  </si>
+  <si>
+    <t>"All-P-uses testing" is not explicitly defined</t>
+  </si>
+  <si>
+    <t>A explicit definition of "all-C-uses testing" should be added</t>
+  </si>
+  <si>
+    <t>A explicit definition of "all-P-uses testing" should be added</t>
+  </si>
+  <si>
+    <t>The word "his/her" is used with no person previously described in this section</t>
+  </si>
+  <si>
+    <t>"…its context and the tester's experience and…"</t>
+  </si>
+  <si>
+    <t>3.3. Experience-Based Techniques</t>
+  </si>
+  <si>
+    <t>Line 4</t>
+  </si>
+  <si>
+    <t>3.3.3. Further Experience-Based Techniques</t>
+  </si>
+  <si>
+    <t>p. 5-14</t>
+  </si>
+  <si>
+    <t>What is the difference between "monkey testing" and "fuzz testing" (see No. 25); is it just that monkey testing's desired effect of is the halting of the program's execution? Is it then a subset of fuzz testing?</t>
+  </si>
+  <si>
+    <t>The distinction between "monkey testing" and "fuzz testing" should be elaborated on</t>
+  </si>
+  <si>
+    <t>The definition of "buddy testing" seems vague; where does the "buddy" part come into play? How is it different from pair testing?</t>
+  </si>
+  <si>
+    <t>The definition of "buddy testing" should be more rigorous</t>
+  </si>
+  <si>
+    <t>Para. 5</t>
+  </si>
+  <si>
+    <t>"… Pair testing allows for generating test cases…"</t>
+  </si>
+  <si>
+    <t>Improve clarity</t>
+  </si>
+  <si>
+    <t> "…test cases with broader and better test coverage."</t>
+  </si>
+  <si>
+    <t>Lines 4-5</t>
+  </si>
+  <si>
+    <t>Lines 5-6</t>
+  </si>
+  <si>
+    <t>Improve consistency</t>
+  </si>
+  <si>
+    <t>Para. 7</t>
+  </si>
+  <si>
+    <t>The purpose of quick testing is unclear; how can "a very small test suite" provide a guarantee of something? I'm assuming the "SUT components that are not fully operational" are what would be the target of this testing?</t>
+  </si>
+  <si>
+    <t>Improve definition/description of "quick testing"</t>
+  </si>
+  <si>
+    <t>Are knowledge-based testing and ML-based testing actual testing techniques, or do they just outline where information that can be used to test can be obtained? This seems like a trivial distinction (e.g., why not "literature-based testing" or "encyclopedia-based testing"?) to make.</t>
+  </si>
+  <si>
+    <t>Either define these test "techniques" more rigorously, move them to a more appropriate section, or remove them entirely</t>
+  </si>
+  <si>
+    <t>How are knowledge-based testing and ML-based testing different?</t>
+  </si>
+  <si>
+    <t>A distinction between "knowledge-based testing" and "ML-based testing" should be added</t>
+  </si>
+  <si>
+    <t>Line 2</t>
+  </si>
+  <si>
+    <t>"Exploit" has negative connotations that likely aren't intentional here</t>
+  </si>
+  <si>
+    <t>"Knowledge-based testing and ML-based testing use (formal or informal) knowledge…"</t>
+  </si>
+  <si>
+    <t>3.5. Usage-Based Techniques</t>
+  </si>
+  <si>
+    <t>p. 5-15</t>
+  </si>
+  <si>
+    <t>Was the omission of "operational testing" as a form of testing intentional?</t>
+  </si>
+  <si>
+    <t>Include and define "operational testing", perhaps using the definition from SWEBOK v3.0 on p. 4-6</t>
+  </si>
+  <si>
+    <t>I'm not sure that this section on combining functional and structural is beneficial. I don't think anyone assumes that one would use only use tests at one phase, for example; would people really think about just using functional or structural testing?</t>
+  </si>
+  <si>
+    <t>Either elaborate on this section to explain some often-misunderstood or confusing way in which these two categories of testing intersect, or remove this section entirely</t>
+  </si>
+  <si>
+    <t>3.7.1. Combining Functional and Structural</t>
+  </si>
+  <si>
+    <t>p.  5-16</t>
+  </si>
+  <si>
+    <t>3.7.2. Deterministic vs. Random</t>
+  </si>
+  <si>
+    <t>"Combining different testing techniques" seems to be the focus of this section (3.7. Selecting and Combining Techniques), but no information about how deterministic and random testing would be combined</t>
+  </si>
+  <si>
+    <t>Provide information on how deterministic and random testing can be combined</t>
+  </si>
+  <si>
+    <t>Is there a better place for this section? It seems to focus more on the method of determining the source of input test data as opposed to the specifics of how testing is performed</t>
+  </si>
+  <si>
+    <t>Move this section to a more logical place, such as 1.2. Key Issues (or one of its children from No. 7)</t>
+  </si>
+  <si>
+    <t>The claim is made that "Several analytical and empirical comparisons have been conducted to analyze the conditions that make one approach more effective than the other," but no examples (or their results!) are given</t>
+  </si>
+  <si>
+    <t>Provide examples of and results from some of these "analytical and empirical comparisons" between deterministic and random testing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Following from No. 47, it is unclear if "deterministic testing" is a specific type of testing (akin to "random testing") or just a way of determining the input data used when using </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> testing techniques (suggested by the lack of use of the term "deterministic testing" in ISO)</t>
+    </r>
+  </si>
+  <si>
+    <t>Either add the definition of "deterministic testing" or make it explicit that while test inputs, etc. can be "selected in a deterministic way", it is always accompanied by a "full-fledged" technique</t>
+  </si>
+  <si>
+    <t>Samuel J. Crawford</t>
   </si>
 </sst>
 </file>
@@ -713,7 +973,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -824,6 +1084,35 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -951,10 +1240,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1247,11 +1532,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1308,16 +1593,16 @@
     </row>
     <row r="2" spans="1:12" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="15">
         <v>1</v>
@@ -1329,26 +1614,34 @@
         <v>47</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="19"/>
+      <c r="A3" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E3" s="15">
         <v>2</v>
       </c>
@@ -1362,17 +1655,25 @@
       <c r="I3" s="16"/>
       <c r="J3" s="31"/>
       <c r="K3" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E4" s="15">
         <v>3</v>
       </c>
@@ -1383,26 +1684,34 @@
         <v>47</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E5" s="15">
         <v>4</v>
       </c>
@@ -1413,26 +1722,34 @@
         <v>47</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>69</v>
-      </c>
       <c r="J5" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E6" s="15">
         <v>5</v>
       </c>
@@ -1443,26 +1760,34 @@
         <v>26</v>
       </c>
       <c r="H6" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E7" s="15">
         <v>6</v>
       </c>
@@ -1473,26 +1798,34 @@
         <v>30</v>
       </c>
       <c r="H7" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="L7" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E8" s="15">
         <v>7</v>
       </c>
@@ -1503,22 +1836,30 @@
         <v>30</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E9" s="15">
         <v>8</v>
       </c>
@@ -1529,24 +1870,32 @@
         <v>30</v>
       </c>
       <c r="H9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="J9" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E10" s="15">
         <v>9</v>
       </c>
@@ -1557,26 +1906,34 @@
         <v>30</v>
       </c>
       <c r="H10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="J10" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="L10" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E11" s="15">
         <v>10</v>
       </c>
@@ -1587,24 +1944,32 @@
         <v>30</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E12" s="15">
         <v>11</v>
       </c>
@@ -1615,26 +1980,34 @@
         <v>30</v>
       </c>
       <c r="H12" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="L12" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E13" s="15">
         <v>12</v>
       </c>
@@ -1645,24 +2018,32 @@
         <v>30</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E14" s="15">
         <v>13</v>
       </c>
@@ -1673,24 +2054,32 @@
         <v>30</v>
       </c>
       <c r="H14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>98</v>
-      </c>
       <c r="K14" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L14" s="17"/>
     </row>
     <row r="15" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="19"/>
+      <c r="A15" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E15" s="15">
         <v>14</v>
       </c>
@@ -1701,22 +2090,30 @@
         <v>30</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>102</v>
-      </c>
       <c r="L15" s="17"/>
     </row>
     <row r="16" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E16" s="15">
         <v>15</v>
       </c>
@@ -1730,17 +2127,25 @@
       <c r="I16" s="16"/>
       <c r="J16" s="31"/>
       <c r="K16" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E17" s="15">
         <v>16</v>
       </c>
@@ -1751,26 +2156,34 @@
         <v>30</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J17" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="L17" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="L17" s="17" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="18" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E18" s="15">
         <v>17</v>
       </c>
@@ -1781,26 +2194,34 @@
         <v>30</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="19"/>
+      <c r="A19" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E19" s="15">
         <v>18</v>
       </c>
@@ -1811,26 +2232,34 @@
         <v>30</v>
       </c>
       <c r="H19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="L19" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E20" s="15">
         <v>19</v>
       </c>
@@ -1841,26 +2270,34 @@
         <v>30</v>
       </c>
       <c r="H20" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="J20" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="K20" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="L20" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="L20" s="17" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="21" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="19"/>
+      <c r="A21" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E21" s="15">
         <v>20</v>
       </c>
@@ -1871,26 +2308,34 @@
         <v>30</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K21" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L21" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="L21" s="17" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="22" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E22" s="15">
         <v>21</v>
       </c>
@@ -1901,26 +2346,34 @@
         <v>30</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I22" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="J22" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="K22" s="17" t="s">
+      <c r="L22" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="L22" s="17" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="23" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="19"/>
+      <c r="A23" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E23" s="15">
         <v>22</v>
       </c>
@@ -1931,462 +2384,1242 @@
         <v>30</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="19"/>
+      <c r="A24" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E24" s="15">
         <v>23</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
+      <c r="F24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E25" s="15">
         <v>24</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="19"/>
+      <c r="F25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="J25" s="31"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="K25" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E26" s="15">
         <v>25</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="19"/>
+      <c r="F26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
       <c r="J26" s="31"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="K26" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E27" s="15">
         <v>26</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="16"/>
+      <c r="F27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="I27" s="16"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="J27" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="19"/>
+      <c r="A28" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E28" s="15">
         <v>27</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="I28" s="16"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="J28" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="19"/>
+      <c r="A29" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E29" s="15">
         <v>28</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="16"/>
+      <c r="F29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="I29" s="16"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="J29" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="19"/>
+      <c r="A30" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E30" s="15">
         <v>29</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="16"/>
+      <c r="F30" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="I30" s="16"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="J30" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="19"/>
+      <c r="A31" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E31" s="15">
         <v>30</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="16"/>
+      <c r="F31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="I31" s="16"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
+      <c r="J31" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="19"/>
+      <c r="A32" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E32" s="15">
         <v>31</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="16"/>
+      <c r="F32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="I32" s="16"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="J32" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="19"/>
+      <c r="A33" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E33" s="15">
         <v>32</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="16"/>
+      <c r="F33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="I33" s="16"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="J33" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="19"/>
+      <c r="A34" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E34" s="15">
         <v>33</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="16"/>
+      <c r="F34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="I34" s="16"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
+      <c r="J34" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="19"/>
+      <c r="A35" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E35" s="15">
         <v>34</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="16"/>
+      <c r="F35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="I35" s="16"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
+      <c r="J35" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="19"/>
+      <c r="A36" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E36" s="15">
         <v>35</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
+      <c r="F36" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="19"/>
+      <c r="A37" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E37" s="15">
         <v>36</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
+      <c r="F37" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="19"/>
+      <c r="A38" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E38" s="15">
         <v>37</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
+      <c r="F38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="19"/>
+      <c r="A39" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E39" s="15">
         <v>38</v>
       </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
+      <c r="F39" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="19"/>
+      <c r="A40" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E40" s="15">
         <v>39</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
+      <c r="F40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="56.5" customHeight="1">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="19"/>
+      <c r="A41" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="E41" s="15">
         <v>40</v>
       </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="G42" s="20"/>
-      <c r="J42" s="32"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="G43" s="20"/>
-      <c r="J43" s="32"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="G44" s="20"/>
-      <c r="J44" s="32"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="G45" s="20"/>
-      <c r="J45" s="32"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="G46" s="20"/>
-      <c r="J46" s="32"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="G47" s="20"/>
-      <c r="J47" s="32"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="G48" s="20"/>
-      <c r="J48" s="32"/>
-    </row>
-    <row r="49" spans="7:10">
-      <c r="G49" s="20"/>
-      <c r="J49" s="32"/>
-    </row>
-    <row r="50" spans="7:10">
-      <c r="G50" s="20"/>
-      <c r="J50" s="32"/>
-    </row>
-    <row r="51" spans="7:10">
-      <c r="G51" s="20"/>
-      <c r="J51" s="32"/>
-    </row>
-    <row r="52" spans="7:10">
-      <c r="G52" s="20"/>
-      <c r="J52" s="32"/>
-    </row>
-    <row r="53" spans="7:10">
-      <c r="G53" s="20"/>
-      <c r="J53" s="32"/>
-    </row>
-    <row r="54" spans="7:10">
-      <c r="G54" s="20"/>
-      <c r="J54" s="32"/>
-    </row>
-    <row r="55" spans="7:10">
-      <c r="G55" s="20"/>
-      <c r="J55" s="32"/>
-    </row>
-    <row r="56" spans="7:10">
-      <c r="G56" s="20"/>
-      <c r="J56" s="32"/>
-    </row>
-    <row r="57" spans="7:10">
-      <c r="G57" s="20"/>
-      <c r="J57" s="32"/>
-    </row>
-    <row r="58" spans="7:10">
-      <c r="G58" s="20"/>
-      <c r="J58" s="32"/>
-    </row>
-    <row r="59" spans="7:10">
-      <c r="G59" s="20"/>
-      <c r="J59" s="32"/>
-    </row>
-    <row r="60" spans="7:10">
-      <c r="G60" s="20"/>
-      <c r="J60" s="32"/>
-    </row>
-    <row r="61" spans="7:10">
-      <c r="G61" s="20"/>
-      <c r="J61" s="32"/>
-    </row>
-    <row r="62" spans="7:10">
-      <c r="G62" s="20"/>
-      <c r="J62" s="32"/>
-    </row>
-    <row r="63" spans="7:10">
-      <c r="G63" s="20"/>
-      <c r="J63" s="32"/>
-    </row>
-    <row r="64" spans="7:10">
-      <c r="G64" s="20"/>
-      <c r="J64" s="32"/>
-    </row>
-    <row r="65" spans="7:10">
-      <c r="G65" s="20"/>
-      <c r="J65" s="32"/>
-    </row>
-    <row r="66" spans="7:10">
+      <c r="F41" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A42" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="15">
+        <v>41</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J42" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A43" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="15">
+        <v>42</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A44" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="15">
+        <v>43</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J44" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A45" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="15">
+        <v>44</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I45" s="16"/>
+      <c r="J45" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="L45" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A46" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="15">
+        <v>45</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I46" s="16"/>
+      <c r="J46" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A47" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="15">
+        <v>46</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K47" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="L47" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A48" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="15">
+        <v>47</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I48" s="16"/>
+      <c r="J48" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="56.25" customHeight="1">
+      <c r="A49" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="15">
+        <v>48</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="56.25" customHeight="1">
+      <c r="A50" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="15">
+        <v>49</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I50" s="16"/>
+      <c r="J50" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D51" s="37"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="42"/>
+      <c r="M51" s="43"/>
+    </row>
+    <row r="52" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D52" s="37"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="43"/>
+    </row>
+    <row r="53" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D53" s="37"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="43"/>
+    </row>
+    <row r="54" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D54" s="37"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="43"/>
+    </row>
+    <row r="55" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D55" s="37"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="41"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="43"/>
+    </row>
+    <row r="56" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D56" s="37"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="41"/>
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="M56" s="43"/>
+    </row>
+    <row r="57" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D57" s="37"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="41"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="43"/>
+    </row>
+    <row r="58" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D58" s="37"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="43"/>
+    </row>
+    <row r="59" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D59" s="37"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="41"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="43"/>
+    </row>
+    <row r="60" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D60" s="37"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="40"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="42"/>
+      <c r="M60" s="43"/>
+    </row>
+    <row r="61" spans="1:13" ht="12.9" customHeight="1">
+      <c r="D61" s="37"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="40"/>
+      <c r="J61" s="41"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
+      <c r="M61" s="43"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="D62" s="37"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="42"/>
+      <c r="M62" s="43"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="42"/>
+      <c r="M63" s="43"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="D64" s="37"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="43"/>
+    </row>
+    <row r="65" spans="4:13">
+      <c r="D65" s="37"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="42"/>
+      <c r="M65" s="43"/>
+    </row>
+    <row r="66" spans="4:13">
       <c r="G66" s="20"/>
       <c r="J66" s="32"/>
     </row>
-    <row r="67" spans="7:10">
+    <row r="67" spans="4:13">
       <c r="G67" s="20"/>
       <c r="J67" s="32"/>
     </row>
-    <row r="68" spans="7:10">
+    <row r="68" spans="4:13">
       <c r="G68" s="20"/>
       <c r="J68" s="32"/>
     </row>
-    <row r="69" spans="7:10">
+    <row r="69" spans="4:13">
       <c r="G69" s="20"/>
       <c r="J69" s="32"/>
     </row>
-    <row r="70" spans="7:10">
+    <row r="70" spans="4:13">
       <c r="G70" s="20"/>
       <c r="J70" s="32"/>
     </row>
-    <row r="71" spans="7:10">
+    <row r="71" spans="4:13">
       <c r="G71" s="20"/>
       <c r="J71" s="32"/>
     </row>
-    <row r="72" spans="7:10">
+    <row r="72" spans="4:13">
       <c r="G72" s="20"/>
       <c r="J72" s="32"/>
     </row>
-    <row r="73" spans="7:10">
+    <row r="73" spans="4:13">
       <c r="G73" s="20"/>
       <c r="J73" s="32"/>
     </row>
-    <row r="74" spans="7:10">
+    <row r="74" spans="4:13">
       <c r="G74" s="20"/>
       <c r="J74" s="32"/>
     </row>
-    <row r="75" spans="7:10">
+    <row r="75" spans="4:13">
       <c r="G75" s="20"/>
       <c r="J75" s="32"/>
     </row>
-    <row r="76" spans="7:10">
+    <row r="76" spans="4:13">
       <c r="G76" s="20"/>
       <c r="J76" s="32"/>
     </row>
-    <row r="77" spans="7:10">
+    <row r="77" spans="4:13">
       <c r="G77" s="20"/>
       <c r="J77" s="32"/>
     </row>
-    <row r="78" spans="7:10">
+    <row r="78" spans="4:13">
       <c r="G78" s="20"/>
       <c r="J78" s="32"/>
     </row>
-    <row r="79" spans="7:10">
+    <row r="79" spans="4:13">
       <c r="G79" s="20"/>
       <c r="J79" s="32"/>
     </row>
-    <row r="80" spans="7:10">
+    <row r="80" spans="4:13">
       <c r="G80" s="20"/>
       <c r="J80" s="32"/>
     </row>
@@ -2589,7 +3822,7 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D41" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F806" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2599,10 +3832,58 @@
   <hyperlinks>
     <hyperlink ref="F1" location="Categories!A1" display="Category" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B84A6E94-19F9-446F-BF82-22DFCF5DD072}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8A02A086-AA3C-42BB-9D34-BA48D5D8A09C}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{B8895358-D773-47A4-9629-6FE8D9DC614B}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{DD4FE001-962A-4062-B911-BB286CABAB0E}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{FEE7AE5A-7B7B-4442-8EF1-D9EB658A8107}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{012F9752-C375-4149-99B8-AB79F5104BEF}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{F29C37A4-A411-4451-9AC7-2A0616D68B65}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{9013E4AC-5B1E-4E18-B860-7A2839216704}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{50B52F5B-C820-4B7E-81C2-6631EB0A09DE}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{527C29BA-F962-4E19-BF69-C0DE35A570C3}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{1CEA901E-074E-4FEA-8D75-11BBAE0F6039}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{1705A78F-C99C-4273-8CF6-A907B9FD5571}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{5753A762-D0C1-4E95-855F-069C045A4003}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{D66A2806-2E9D-4FA6-999F-6CA0B2E81313}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{94F04975-1BB5-4760-A85B-852D133CF81A}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{04A343C3-A450-404E-9034-50757F6D0A3B}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{DFF7A62A-2500-49B5-A5AA-884105928DEB}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{87D79CAA-1348-4CEE-8A54-A00EAA9CC70F}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{6CD8079A-17E9-4BB9-B589-96E42AB550E8}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{C556D95B-CFCB-4DDB-AE27-ACB63A9AFC73}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{075616B2-5C6B-4EE1-9022-BBCDDE1013DE}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{1BAE4B30-2B49-4D05-BD79-DC31DCF3FE6D}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{64032637-E7BD-4339-B213-D29FFACB6CB0}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{9DA73F13-ADDE-4F1E-A4B7-C285F9717E0E}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{643AA8A2-19AE-435C-8606-6EBEF15B4F2F}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{7A2B6A93-D423-4E12-B5FB-E1E926CA9925}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{50E6469A-8443-4015-A27A-4D20B308685F}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{666F5EE8-D315-40BE-8AB9-9C89C10F05D4}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{F03242CF-EBF9-4186-AEED-DE8CCA30603D}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{7D350C60-2294-4BCC-BA9A-96045709440C}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{91107F84-2DEE-4C6D-8E5A-443BB90C16AF}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{20A4A3CF-6419-4F56-BBC2-A60A5BA4D103}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{7CA4EB39-84FE-4ED6-AE6D-30C9546D5A19}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{99A789A5-7679-4179-BE47-D1B3EFD14A34}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{A1FD8956-37F6-41AA-979C-87345718DE2F}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{6160D7FB-5B57-4783-9E12-C8DF187371FB}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{BD97063A-C51C-4B05-8408-6F9041B6DCE9}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{0C7648FD-6EFC-40E9-B4F2-0B630D3CA6DE}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{4DB475CA-58E2-430C-B934-D644B122E7B8}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{DA054CB3-BEE7-416A-8462-2D981C5DD018}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{A0B4C842-50E7-4454-A40C-D907A09C850F}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{E6896414-D27B-4BC6-B025-2593377B39CC}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{CD3C9C60-8A34-4170-A1C0-909DCF74DB68}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{FD52B809-39C0-4B3F-B73D-1FC1107D23D4}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{70478C29-C394-42B4-832A-BDA3A43CB2F2}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{8BE51798-9F28-4E6B-AD59-8D5A3887BD54}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{511DD410-6A69-43A8-8F3A-CAE2A8C507A0}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{F5B11D4C-86B2-48A4-96EC-35EA58FD9BD3}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{C2E5014C-5035-4F57-8116-A29BF9082082}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId50"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -2615,7 +3896,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G41</xm:sqref>
+          <xm:sqref>G2:G61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fill in 'Proposed new text' column as done in last commit
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663CC136-25DF-459E-A583-D17E027687FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8FC9B-C4A4-44BA-8C3E-C6F01EF71D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="208">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -475,9 +475,6 @@
     <t>Line 3</t>
   </si>
   <si>
-    <t>Subsections 1-6, 10, 12, and 14 of Section 1.2 Key Issues seem to focus more on "areas for consideration" or "topics" of testing than actual "issues"; could this section be split into two, one of actual issues and one of these "areas for consideration"?</t>
-  </si>
-  <si>
     <t>1.2.15. Off-Line vs. Online Testing</t>
   </si>
   <si>
@@ -839,6 +836,27 @@
   </si>
   <si>
     <t>Samuel J. Crawford</t>
+  </si>
+  <si>
+    <t>Elaborate on what it means to "manag[e] the infeasible paths"</t>
+  </si>
+  <si>
+    <t>Move this section to 3.7. Selecting and Combining Techniques</t>
+  </si>
+  <si>
+    <t>Either correct what actually "can improve accuracy", or remove "and can improve accuracy" from this sentence</t>
+  </si>
+  <si>
+    <t>"…are important considerations to make when software testing…"</t>
+  </si>
+  <si>
+    <t>Elaborate on how "specifications, behavioral models, and code annotations" can function as oracles; and define/described "mechanized oracles"</t>
+  </si>
+  <si>
+    <t>Subsections 1-6, 10, 12, and 14 of Section 1.2 Key Issues seem to focus more on "areas for consideration" or "topics" of testing than actual "issues"</t>
+  </si>
+  <si>
+    <t>Split this section into two: one section describing actual issues with testing and another to describe these "areas for consideration"</t>
   </si>
 </sst>
 </file>
@@ -973,7 +991,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1076,6 +1094,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1084,35 +1110,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1532,11 +1529,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1593,7 +1590,7 @@
     </row>
     <row r="2" spans="1:12" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>56</v>
@@ -1631,7 +1628,7 @@
     </row>
     <row r="3" spans="1:12" ht="56.5" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>56</v>
@@ -1663,7 +1660,7 @@
     </row>
     <row r="4" spans="1:12" ht="56.5" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>56</v>
@@ -1701,7 +1698,7 @@
     </row>
     <row r="5" spans="1:12" ht="56.5" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>56</v>
@@ -1739,7 +1736,7 @@
     </row>
     <row r="6" spans="1:12" ht="56.5" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>56</v>
@@ -1777,7 +1774,7 @@
     </row>
     <row r="7" spans="1:12" ht="56.5" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>56</v>
@@ -1815,7 +1812,7 @@
     </row>
     <row r="8" spans="1:12" ht="56.5" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>56</v>
@@ -1843,13 +1840,15 @@
         <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="17"/>
+        <v>206</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="56.5" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>56</v>
@@ -1881,11 +1880,13 @@
       <c r="K9" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="17" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="56.5" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>56</v>
@@ -1923,7 +1924,7 @@
     </row>
     <row r="11" spans="1:12" ht="56.5" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>56</v>
@@ -1955,11 +1956,13 @@
       <c r="K11" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="17"/>
+      <c r="L11" s="17" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="56.5" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>56</v>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="13" spans="1:12" ht="56.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>56</v>
@@ -2029,11 +2032,13 @@
       <c r="K13" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="17"/>
+      <c r="L13" s="17" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="56.5" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>56</v>
@@ -2065,11 +2070,13 @@
       <c r="K14" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="17" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="56.5" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>56</v>
@@ -2090,20 +2097,22 @@
         <v>30</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="17" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="56.5" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>56</v>
@@ -2127,15 +2136,15 @@
       <c r="I16" s="16"/>
       <c r="J16" s="31"/>
       <c r="K16" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="56.5" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>56</v>
@@ -2156,24 +2165,24 @@
         <v>30</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J17" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="L17" s="17" t="s">
         <v>105</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="56.5" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>56</v>
@@ -2194,7 +2203,7 @@
         <v>30</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>87</v>
@@ -2203,15 +2212,15 @@
         <v>97</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="56.5" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>56</v>
@@ -2232,24 +2241,24 @@
         <v>30</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="56.5" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>56</v>
@@ -2270,24 +2279,24 @@
         <v>30</v>
       </c>
       <c r="H20" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="J20" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="K20" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="L20" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="56.5" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>56</v>
@@ -2308,24 +2317,24 @@
         <v>30</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="L21" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="L21" s="17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="56.5" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>56</v>
@@ -2346,24 +2355,24 @@
         <v>30</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I22" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="J22" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="17" t="s">
+      <c r="L22" s="17" t="s">
         <v>122</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="56.5" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>56</v>
@@ -2384,24 +2393,24 @@
         <v>30</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="56.5" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>56</v>
@@ -2422,7 +2431,7 @@
         <v>30</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>87</v>
@@ -2431,15 +2440,15 @@
         <v>97</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="56.5" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>56</v>
@@ -2463,15 +2472,15 @@
       <c r="I25" s="16"/>
       <c r="J25" s="31"/>
       <c r="K25" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="56.5" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>56</v>
@@ -2495,15 +2504,15 @@
       <c r="I26" s="16"/>
       <c r="J26" s="31"/>
       <c r="K26" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="56.5" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>56</v>
@@ -2524,22 +2533,22 @@
         <v>30</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="56.5" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>56</v>
@@ -2560,22 +2569,22 @@
         <v>30</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K28" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L28" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="56.5" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>56</v>
@@ -2596,22 +2605,22 @@
         <v>30</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="56.5" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>56</v>
@@ -2632,22 +2641,22 @@
         <v>30</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="56.5" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>56</v>
@@ -2668,22 +2677,22 @@
         <v>30</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K31" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="L31" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="56.5" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>56</v>
@@ -2704,22 +2713,22 @@
         <v>30</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K32" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L32" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="56.5" customHeight="1">
       <c r="A33" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>56</v>
@@ -2740,22 +2749,22 @@
         <v>30</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="56.5" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>56</v>
@@ -2776,22 +2785,22 @@
         <v>30</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="56.5" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>56</v>
@@ -2812,22 +2821,22 @@
         <v>30</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K35" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="L35" s="17" t="s">
         <v>151</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="56.5" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>56</v>
@@ -2848,24 +2857,24 @@
         <v>30</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K36" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="L36" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="56.5" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>56</v>
@@ -2886,24 +2895,24 @@
         <v>30</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="J37" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="L37" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="56.5" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>56</v>
@@ -2924,24 +2933,24 @@
         <v>30</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K38" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L38" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="56.5" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>56</v>
@@ -2962,24 +2971,24 @@
         <v>30</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I39" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="L39" s="17" t="s">
         <v>167</v>
-      </c>
-      <c r="J39" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="56.5" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>56</v>
@@ -3000,24 +3009,24 @@
         <v>30</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J40" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="K40" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="K40" s="17" t="s">
-        <v>173</v>
-      </c>
       <c r="L40" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="56.5" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>56</v>
@@ -3038,24 +3047,24 @@
         <v>30</v>
       </c>
       <c r="H41" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="J41" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="K41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="J41" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="K41" s="17" t="s">
+      <c r="L41" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="56.25" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>56</v>
@@ -3076,24 +3085,24 @@
         <v>30</v>
       </c>
       <c r="H42" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="I42" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="J42" s="31" t="s">
-        <v>162</v>
-      </c>
       <c r="K42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L42" s="17" t="s">
         <v>177</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="56.25" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>56</v>
@@ -3114,24 +3123,24 @@
         <v>30</v>
       </c>
       <c r="H43" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J43" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="I43" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="J43" s="31" t="s">
-        <v>162</v>
-      </c>
       <c r="K43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L43" s="17" t="s">
         <v>179</v>
-      </c>
-      <c r="L43" s="17" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="56.25" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>56</v>
@@ -3152,24 +3161,24 @@
         <v>30</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J44" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="K44" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="L44" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="56.25" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>56</v>
@@ -3190,22 +3199,22 @@
         <v>30</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="K45" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="L45" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="56.25" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" s="29" t="s">
         <v>56</v>
@@ -3226,22 +3235,22 @@
         <v>30</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K46" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="L46" s="17" t="s">
         <v>188</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="56.25" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>56</v>
@@ -3262,22 +3271,22 @@
         <v>30</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K47" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="L47" s="17" t="s">
         <v>193</v>
-      </c>
-      <c r="L47" s="17" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="56.25" customHeight="1">
       <c r="A48" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B48" s="29" t="s">
         <v>56</v>
@@ -3298,22 +3307,22 @@
         <v>30</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K48" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="L48" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="L48" s="17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="56.25" customHeight="1">
+    </row>
+    <row r="49" spans="1:12" ht="56.25" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>56</v>
@@ -3334,22 +3343,22 @@
         <v>30</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I49" s="16"/>
       <c r="J49" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K49" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="L49" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="L49" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="56.25" customHeight="1">
+    </row>
+    <row r="50" spans="1:12" ht="56.25" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>56</v>
@@ -3370,256 +3379,136 @@
         <v>30</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I50" s="16"/>
       <c r="J50" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K50" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="L50" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="L50" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D51" s="37"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="43"/>
-    </row>
-    <row r="52" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D52" s="37"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="41"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="43"/>
-    </row>
-    <row r="53" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="43"/>
-    </row>
-    <row r="54" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="43"/>
-    </row>
-    <row r="55" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D55" s="37"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="43"/>
-    </row>
-    <row r="56" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="42"/>
-      <c r="L56" s="42"/>
-      <c r="M56" s="43"/>
-    </row>
-    <row r="57" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D57" s="37"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="42"/>
-      <c r="L57" s="42"/>
-      <c r="M57" s="43"/>
-    </row>
-    <row r="58" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D58" s="37"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="42"/>
-      <c r="L58" s="42"/>
-      <c r="M58" s="43"/>
-    </row>
-    <row r="59" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D59" s="37"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="43"/>
-    </row>
-    <row r="60" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D60" s="37"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="42"/>
-      <c r="L60" s="42"/>
-      <c r="M60" s="43"/>
-    </row>
-    <row r="61" spans="1:13" ht="12.9" customHeight="1">
-      <c r="D61" s="37"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="42"/>
-      <c r="M61" s="43"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="44"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="45"/>
-      <c r="K62" s="42"/>
-      <c r="L62" s="42"/>
-      <c r="M62" s="43"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="D63" s="37"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="42"/>
-      <c r="L63" s="42"/>
-      <c r="M63" s="43"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="D64" s="37"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="42"/>
-      <c r="L64" s="42"/>
-      <c r="M64" s="43"/>
-    </row>
-    <row r="65" spans="4:13">
-      <c r="D65" s="37"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="45"/>
-      <c r="K65" s="42"/>
-      <c r="L65" s="42"/>
-      <c r="M65" s="43"/>
-    </row>
-    <row r="66" spans="4:13">
+    </row>
+    <row r="51" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G51" s="34"/>
+      <c r="J51" s="35"/>
+    </row>
+    <row r="52" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G52" s="34"/>
+      <c r="J52" s="35"/>
+    </row>
+    <row r="53" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G53" s="34"/>
+      <c r="J53" s="35"/>
+    </row>
+    <row r="54" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G54" s="34"/>
+      <c r="J54" s="35"/>
+    </row>
+    <row r="55" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G55" s="34"/>
+      <c r="J55" s="35"/>
+    </row>
+    <row r="56" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G56" s="34"/>
+      <c r="J56" s="35"/>
+    </row>
+    <row r="57" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G57" s="34"/>
+      <c r="J57" s="35"/>
+    </row>
+    <row r="58" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G58" s="34"/>
+      <c r="J58" s="35"/>
+    </row>
+    <row r="59" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G59" s="34"/>
+      <c r="J59" s="35"/>
+    </row>
+    <row r="60" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G60" s="34"/>
+      <c r="J60" s="35"/>
+    </row>
+    <row r="61" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G61" s="34"/>
+      <c r="J61" s="35"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="G62" s="20"/>
+      <c r="J62" s="32"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="G63" s="20"/>
+      <c r="J63" s="32"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="G64" s="20"/>
+      <c r="J64" s="32"/>
+    </row>
+    <row r="65" spans="7:10">
+      <c r="G65" s="20"/>
+      <c r="J65" s="32"/>
+    </row>
+    <row r="66" spans="7:10">
       <c r="G66" s="20"/>
       <c r="J66" s="32"/>
     </row>
-    <row r="67" spans="4:13">
+    <row r="67" spans="7:10">
       <c r="G67" s="20"/>
       <c r="J67" s="32"/>
     </row>
-    <row r="68" spans="4:13">
+    <row r="68" spans="7:10">
       <c r="G68" s="20"/>
       <c r="J68" s="32"/>
     </row>
-    <row r="69" spans="4:13">
+    <row r="69" spans="7:10">
       <c r="G69" s="20"/>
       <c r="J69" s="32"/>
     </row>
-    <row r="70" spans="4:13">
+    <row r="70" spans="7:10">
       <c r="G70" s="20"/>
       <c r="J70" s="32"/>
     </row>
-    <row r="71" spans="4:13">
+    <row r="71" spans="7:10">
       <c r="G71" s="20"/>
       <c r="J71" s="32"/>
     </row>
-    <row r="72" spans="4:13">
+    <row r="72" spans="7:10">
       <c r="G72" s="20"/>
       <c r="J72" s="32"/>
     </row>
-    <row r="73" spans="4:13">
+    <row r="73" spans="7:10">
       <c r="G73" s="20"/>
       <c r="J73" s="32"/>
     </row>
-    <row r="74" spans="4:13">
+    <row r="74" spans="7:10">
       <c r="G74" s="20"/>
       <c r="J74" s="32"/>
     </row>
-    <row r="75" spans="4:13">
+    <row r="75" spans="7:10">
       <c r="G75" s="20"/>
       <c r="J75" s="32"/>
     </row>
-    <row r="76" spans="4:13">
+    <row r="76" spans="7:10">
       <c r="G76" s="20"/>
       <c r="J76" s="32"/>
     </row>
-    <row r="77" spans="4:13">
+    <row r="77" spans="7:10">
       <c r="G77" s="20"/>
       <c r="J77" s="32"/>
     </row>
-    <row r="78" spans="4:13">
+    <row r="78" spans="7:10">
       <c r="G78" s="20"/>
       <c r="J78" s="32"/>
     </row>
-    <row r="79" spans="4:13">
+    <row r="79" spans="7:10">
       <c r="G79" s="20"/>
       <c r="J79" s="32"/>
     </row>
-    <row r="80" spans="4:13">
+    <row r="80" spans="7:10">
       <c r="G80" s="20"/>
       <c r="J80" s="32"/>
     </row>
@@ -3999,11 +3888,11 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="42.75" customHeight="1">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="9" t="s">
@@ -4011,11 +3900,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="35.25" customHeight="1">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="9" t="s">
@@ -4023,11 +3912,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="57" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
@@ -4035,11 +3924,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="47.25" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
@@ -4047,11 +3936,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="57.75" customHeight="1">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Improve consistency of feedback
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8FC9B-C4A4-44BA-8C3E-C6F01EF71D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA8E752-95C0-4EC2-9E76-2D7193DD8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="208">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -603,21 +603,12 @@
     <t>2.2.10. Interface and Application Program Interface (API) Testing</t>
   </si>
   <si>
-    <t>"Boundary value analysis" and "all combinations testing" throughout the document</t>
-  </si>
-  <si>
     <t>"Fuzz testing" is the more common term used for what is called "fuzzy testing"; for example, ISO/IEC/IEEE 29119-1:2022 only uses the former</t>
   </si>
   <si>
     <t>Should "Boundary-Value Analysis" and "All-Combinations Testing" have hyphens or no? They don't in ISO/IEC/IEEE 29119-4:2021, for example (see 3.3 and 3.12, respectively)</t>
   </si>
   <si>
-    <t>"Fuzz testing" throughout the document</t>
-  </si>
-  <si>
-    <t>More detail defining/describing evidence-based testing</t>
-  </si>
-  <si>
     <t>Evidence-based testing isn't really defined/described, just how it applies to software engineering as a whole. What questions would be relevant? What kinds of evidence would be useful? It seems more like a "workflow" for designing other kinds of tests rather than an actual type of testing.</t>
   </si>
   <si>
@@ -741,9 +732,6 @@
     <t>The purpose of quick testing is unclear; how can "a very small test suite" provide a guarantee of something? I'm assuming the "SUT components that are not fully operational" are what would be the target of this testing?</t>
   </si>
   <si>
-    <t>Improve definition/description of "quick testing"</t>
-  </si>
-  <si>
     <t>Are knowledge-based testing and ML-based testing actual testing techniques, or do they just outline where information that can be used to test can be obtained? This seems like a trivial distinction (e.g., why not "literature-based testing" or "encyclopedia-based testing"?) to make.</t>
   </si>
   <si>
@@ -753,9 +741,6 @@
     <t>How are knowledge-based testing and ML-based testing different?</t>
   </si>
   <si>
-    <t>A distinction between "knowledge-based testing" and "ML-based testing" should be added</t>
-  </si>
-  <si>
     <t>Line 2</t>
   </si>
   <si>
@@ -790,12 +775,6 @@
   </si>
   <si>
     <t>3.7.2. Deterministic vs. Random</t>
-  </si>
-  <si>
-    <t>"Combining different testing techniques" seems to be the focus of this section (3.7. Selecting and Combining Techniques), but no information about how deterministic and random testing would be combined</t>
-  </si>
-  <si>
-    <t>Provide information on how deterministic and random testing can be combined</t>
   </si>
   <si>
     <t>Is there a better place for this section? It seems to focus more on the method of determining the source of input test data as opposed to the specifics of how testing is performed</t>
@@ -857,6 +836,27 @@
   </si>
   <si>
     <t>Split this section into two: one section describing actual issues with testing and another to describe these "areas for consideration"</t>
+  </si>
+  <si>
+    <t>"Combining different testing techniques" seems to be the focus of this section (3.7. Selecting and Combining Techniques), but there is no information about how deterministic and random testing would be combined</t>
+  </si>
+  <si>
+    <t>Add information on how deterministic and random testing can be combined</t>
+  </si>
+  <si>
+    <t>"Boundary value analysis" and "all combinations testing" should be used throughout the document</t>
+  </si>
+  <si>
+    <t>"Fuzz testing" should be used throughout the document</t>
+  </si>
+  <si>
+    <t>A more explicit definition/description of evidence-based testing should be added</t>
+  </si>
+  <si>
+    <t>Improve the rigor/coherence of the definition and description of "quick testing"</t>
+  </si>
+  <si>
+    <t>A distinction between "knowledge-based testing" and "ML-based testing" should be made</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1532,8 @@
   <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="2" spans="1:12" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>56</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="3" spans="1:12" ht="56.5" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>56</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="4" spans="1:12" ht="56.5" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>56</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="5" spans="1:12" ht="56.5" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>56</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="6" spans="1:12" ht="56.5" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>56</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="7" spans="1:12" ht="56.5" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>56</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="8" spans="1:12" ht="56.5" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>56</v>
@@ -1840,15 +1840,15 @@
         <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="56.5" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>56</v>
@@ -1881,12 +1881,12 @@
         <v>89</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="56.5" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>56</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="11" spans="1:12" ht="56.5" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>56</v>
@@ -1957,12 +1957,12 @@
         <v>90</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="56.5" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>56</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="13" spans="1:12" ht="56.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>56</v>
@@ -2033,12 +2033,12 @@
         <v>94</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="56.5" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>56</v>
@@ -2071,12 +2071,12 @@
         <v>95</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="56.5" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>56</v>
@@ -2107,12 +2107,12 @@
         <v>100</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="56.5" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>56</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="17" spans="1:12" ht="56.5" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>56</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="18" spans="1:12" ht="56.5" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>56</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="19" spans="1:12" ht="56.5" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>56</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="20" spans="1:12" ht="56.5" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>56</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="21" spans="1:12" ht="56.5" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>56</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="22" spans="1:12" ht="56.5" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>56</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="23" spans="1:12" ht="56.5" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>56</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="24" spans="1:12" ht="56.5" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>56</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="25" spans="1:12" ht="56.5" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>56</v>
@@ -2472,15 +2472,15 @@
       <c r="I25" s="16"/>
       <c r="J25" s="31"/>
       <c r="K25" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>129</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="56.5" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>56</v>
@@ -2504,15 +2504,15 @@
       <c r="I26" s="16"/>
       <c r="J26" s="31"/>
       <c r="K26" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="56.5" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>56</v>
@@ -2533,22 +2533,22 @@
         <v>30</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="56.5" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>56</v>
@@ -2569,22 +2569,22 @@
         <v>30</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="L28" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="56.5" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>56</v>
@@ -2605,22 +2605,22 @@
         <v>30</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="56.5" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>56</v>
@@ -2641,22 +2641,22 @@
         <v>30</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="56.5" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>56</v>
@@ -2677,22 +2677,22 @@
         <v>30</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="56.5" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>56</v>
@@ -2713,22 +2713,22 @@
         <v>30</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="56.5" customHeight="1">
       <c r="A33" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>56</v>
@@ -2749,22 +2749,22 @@
         <v>30</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="56.5" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>56</v>
@@ -2785,22 +2785,22 @@
         <v>30</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="56.5" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>56</v>
@@ -2821,22 +2821,22 @@
         <v>30</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="56.5" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>56</v>
@@ -2857,24 +2857,24 @@
         <v>30</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="56.5" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>56</v>
@@ -2895,24 +2895,24 @@
         <v>30</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="J37" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K37" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="56.5" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>56</v>
@@ -2933,24 +2933,24 @@
         <v>30</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J38" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="K38" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="K38" s="17" t="s">
-        <v>164</v>
-      </c>
       <c r="L38" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="56.5" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>56</v>
@@ -2971,24 +2971,24 @@
         <v>30</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J39" s="31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L39" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="56.5" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>56</v>
@@ -3009,24 +3009,24 @@
         <v>30</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I40" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L40" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="J40" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="K40" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="L40" s="17" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="56.5" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>56</v>
@@ -3047,24 +3047,24 @@
         <v>30</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="56.25" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>56</v>
@@ -3085,24 +3085,24 @@
         <v>30</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="56.25" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>56</v>
@@ -3123,24 +3123,24 @@
         <v>30</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I43" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="56.25" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>56</v>
@@ -3161,24 +3161,24 @@
         <v>30</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I44" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="56.25" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>56</v>
@@ -3199,22 +3199,22 @@
         <v>30</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="31" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K45" s="17" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L45" s="17" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="56.25" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B46" s="29" t="s">
         <v>56</v>
@@ -3235,22 +3235,22 @@
         <v>30</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="56.25" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>56</v>
@@ -3271,22 +3271,22 @@
         <v>30</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="L47" s="17" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="56.25" customHeight="1">
       <c r="A48" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B48" s="29" t="s">
         <v>56</v>
@@ -3307,22 +3307,22 @@
         <v>30</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="L48" s="17" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="56.25" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>56</v>
@@ -3343,22 +3343,24 @@
         <v>30</v>
       </c>
       <c r="H49" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J49" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="K49" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="I49" s="16"/>
-      <c r="J49" s="31" t="s">
-        <v>190</v>
-      </c>
-      <c r="K49" s="17" t="s">
-        <v>198</v>
-      </c>
       <c r="L49" s="17" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="56.25" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>56</v>
@@ -3379,17 +3381,19 @@
         <v>30</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="I50" s="16"/>
+        <v>186</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="J50" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="L50" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="K50" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="L50" s="17" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="12.9" customHeight="1">

</xml_diff>

<commit_message>
Improve consistency of feedback about improving definitions
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA8E752-95C0-4EC2-9E76-2D7193DD8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05D4116-8BF5-49A5-86E7-39C4FC3C1B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,9 +532,6 @@
     <t>"Scalability testing evaluates the capability to use and learn the system and the user documentation. It also focuses on the system's effectiveness in supporting user tasks and the ability to recover from user errors"; this seems to describe usability testing, which evaluates "how easy it is for end-users to learn to use the software" (p. 5-10)</t>
   </si>
   <si>
-    <t>Redefine scalability testing</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -552,9 +549,6 @@
       </rPr>
       <t> by Ian Sommerville is cited as the only source for the section on elasticity testing, but the words "elasticity" and "elastic" don't even show up in the book!</t>
     </r>
-  </si>
-  <si>
-    <t>Find a legitimate definition (with source) for elasticity testing</t>
   </si>
   <si>
     <t>Para. 10</t>
@@ -857,6 +851,12 @@
   </si>
   <si>
     <t>A distinction between "knowledge-based testing" and "ML-based testing" should be made</t>
+  </si>
+  <si>
+    <t>Rename this definition to "usability testing" and add a correct definition for "scalability testing"</t>
+  </si>
+  <si>
+    <t>Add a definition (with a source) for "elasticity testing"</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1532,8 @@
   <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="2" spans="1:12" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>56</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="3" spans="1:12" ht="56.5" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>56</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="4" spans="1:12" ht="56.5" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>56</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="5" spans="1:12" ht="56.5" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>56</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="6" spans="1:12" ht="56.5" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>56</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="7" spans="1:12" ht="56.5" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>56</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="8" spans="1:12" ht="56.5" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>56</v>
@@ -1840,15 +1840,15 @@
         <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="56.5" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>56</v>
@@ -1881,12 +1881,12 @@
         <v>89</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="56.5" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>56</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="11" spans="1:12" ht="56.5" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>56</v>
@@ -1957,12 +1957,12 @@
         <v>90</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="56.5" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>56</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="13" spans="1:12" ht="56.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>56</v>
@@ -2033,12 +2033,12 @@
         <v>94</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="56.5" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>56</v>
@@ -2071,12 +2071,12 @@
         <v>95</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="56.5" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>56</v>
@@ -2107,12 +2107,12 @@
         <v>100</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="56.5" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>56</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="17" spans="1:12" ht="56.5" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>56</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="18" spans="1:12" ht="56.5" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>56</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="19" spans="1:12" ht="56.5" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>56</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="20" spans="1:12" ht="56.5" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>56</v>
@@ -2291,12 +2291,12 @@
         <v>116</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="56.5" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>56</v>
@@ -2320,21 +2320,21 @@
         <v>113</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J21" s="31" t="s">
         <v>115</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="56.5" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>56</v>
@@ -2358,21 +2358,21 @@
         <v>113</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J22" s="31" t="s">
         <v>115</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="56.5" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>56</v>
@@ -2396,21 +2396,21 @@
         <v>113</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J23" s="31" t="s">
         <v>115</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="56.5" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>56</v>
@@ -2431,7 +2431,7 @@
         <v>30</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>87</v>
@@ -2440,15 +2440,15 @@
         <v>97</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="56.5" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>56</v>
@@ -2472,15 +2472,15 @@
       <c r="I25" s="16"/>
       <c r="J25" s="31"/>
       <c r="K25" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="56.5" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>56</v>
@@ -2504,15 +2504,15 @@
       <c r="I26" s="16"/>
       <c r="J26" s="31"/>
       <c r="K26" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="56.5" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>56</v>
@@ -2533,22 +2533,22 @@
         <v>30</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="56.5" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>56</v>
@@ -2569,22 +2569,22 @@
         <v>30</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="K28" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>136</v>
-      </c>
       <c r="L28" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="56.5" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>56</v>
@@ -2605,22 +2605,22 @@
         <v>30</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="56.5" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>56</v>
@@ -2641,22 +2641,22 @@
         <v>30</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="56.5" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>56</v>
@@ -2677,22 +2677,22 @@
         <v>30</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="56.5" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>56</v>
@@ -2713,22 +2713,22 @@
         <v>30</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="56.5" customHeight="1">
       <c r="A33" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>56</v>
@@ -2749,22 +2749,22 @@
         <v>30</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K33" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L33" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="56.5" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>56</v>
@@ -2785,22 +2785,22 @@
         <v>30</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K34" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L34" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="56.5" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>56</v>
@@ -2821,22 +2821,22 @@
         <v>30</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="56.5" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>56</v>
@@ -2857,24 +2857,24 @@
         <v>30</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="56.5" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>56</v>
@@ -2895,24 +2895,24 @@
         <v>30</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="J37" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="L37" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="K37" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="56.5" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>56</v>
@@ -2933,24 +2933,24 @@
         <v>30</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="56.5" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>56</v>
@@ -2971,24 +2971,24 @@
         <v>30</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I39" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="K39" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="J39" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>165</v>
-      </c>
       <c r="L39" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="56.5" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>56</v>
@@ -3009,24 +3009,24 @@
         <v>30</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="56.5" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>56</v>
@@ -3047,24 +3047,24 @@
         <v>30</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="56.25" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>56</v>
@@ -3085,24 +3085,24 @@
         <v>30</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="56.25" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>56</v>
@@ -3123,24 +3123,24 @@
         <v>30</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I43" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="56.25" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>56</v>
@@ -3161,24 +3161,24 @@
         <v>30</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I44" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J44" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L44" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="56.25" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>56</v>
@@ -3199,22 +3199,22 @@
         <v>30</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L45" s="17" t="s">
         <v>179</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="56.25" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B46" s="29" t="s">
         <v>56</v>
@@ -3235,22 +3235,22 @@
         <v>30</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="56.25" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>56</v>
@@ -3271,22 +3271,22 @@
         <v>30</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L47" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="56.25" customHeight="1">
       <c r="A48" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B48" s="29" t="s">
         <v>56</v>
@@ -3307,22 +3307,22 @@
         <v>30</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="K48" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="K48" s="17" t="s">
-        <v>187</v>
-      </c>
       <c r="L48" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="56.25" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>56</v>
@@ -3343,24 +3343,24 @@
         <v>30</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I49" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J49" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="56.25" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>56</v>
@@ -3381,19 +3381,19 @@
         <v>30</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I50" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J50" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L50" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="12.9" customHeight="1">

</xml_diff>

<commit_message>
Add rest of comments on SWEBOK's testing chapter
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05D4116-8BF5-49A5-86E7-39C4FC3C1B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C127815-AFEE-4626-B473-965B0E96B83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="OLE_LINK5" localSheetId="0">Comments!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Comments!$A:$E,Comments!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="217">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -857,6 +857,69 @@
   </si>
   <si>
     <t>Add a definition (with a source) for "elasticity testing"</t>
+  </si>
+  <si>
+    <t>5.2.3. Test Environment Set-up and Maintenance</t>
+  </si>
+  <si>
+    <t>Line 9</t>
+  </si>
+  <si>
+    <t>Replace "in vitro or in vivo" with what that means in the context of software testing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Since the terms "in vitro" and "in vivo" are never used in this document, it is unclear what they mean in the context of software engineering; does this mean that the testing environment can be either the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>actual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> environment or a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>simulated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> one (which seems redudant, since "simulated" is already given)?</t>
+    </r>
+  </si>
+  <si>
+    <t>5.3. Staffing</t>
+  </si>
+  <si>
+    <t>Paras. 1-2</t>
+  </si>
+  <si>
+    <t>Lines 7-8</t>
+  </si>
+  <si>
+    <t>A page break was added erroneously</t>
+  </si>
+  <si>
+    <t>"…to meet deadlines, and increase/reduce maintenance costs." (with no paragraph break)</t>
   </si>
 </sst>
 </file>
@@ -1529,11 +1592,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -3396,13 +3459,81 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G51" s="34"/>
-      <c r="J51" s="35"/>
-    </row>
-    <row r="52" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G52" s="34"/>
-      <c r="J52" s="35"/>
+    <row r="51" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A51" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" s="15">
+        <v>50</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="L51" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A52" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="15">
+        <v>51</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="L52" s="17" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="53" spans="1:12" ht="12.9" customHeight="1">
       <c r="G53" s="34"/>
@@ -3440,9 +3571,9 @@
       <c r="G61" s="34"/>
       <c r="J61" s="35"/>
     </row>
-    <row r="62" spans="1:12">
-      <c r="G62" s="20"/>
-      <c r="J62" s="32"/>
+    <row r="62" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G62" s="34"/>
+      <c r="J62" s="35"/>
     </row>
     <row r="63" spans="1:12">
       <c r="G63" s="20"/>
@@ -3712,13 +3843,17 @@
       <c r="G129" s="20"/>
       <c r="J129" s="32"/>
     </row>
+    <row r="130" spans="7:10">
+      <c r="G130" s="20"/>
+      <c r="J130" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D52" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F806" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F807" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -3773,10 +3908,12 @@
     <hyperlink ref="B48" r:id="rId47" xr:uid="{511DD410-6A69-43A8-8F3A-CAE2A8C507A0}"/>
     <hyperlink ref="B49" r:id="rId48" xr:uid="{F5B11D4C-86B2-48A4-96EC-35EA58FD9BD3}"/>
     <hyperlink ref="B50" r:id="rId49" xr:uid="{C2E5014C-5035-4F57-8116-A29BF9082082}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
+    <hyperlink ref="B51" r:id="rId51" xr:uid="{BA099E17-6C3D-4BDD-8CDF-DABDDB357C20}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId50"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId52"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -3789,7 +3926,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G61</xm:sqref>
+          <xm:sqref>G2:G62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add notes from SWEBOK's section 2. Software Engineering Operations Planning
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C127815-AFEE-4626-B473-965B0E96B83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0955DB07-1FBF-4DBC-B5F1-050A6B4C330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="221">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -920,6 +920,18 @@
   </si>
   <si>
     <t>"…to meet deadlines, and increase/reduce maintenance costs." (with no paragraph break)</t>
+  </si>
+  <si>
+    <t>2.5. Software Backup, Disaster Recovery and Failover</t>
+  </si>
+  <si>
+    <t>Lines 1-6</t>
+  </si>
+  <si>
+    <t>The number of commas makes this sentence not intuitively understandable</t>
+  </si>
+  <si>
+    <t>"ISO/IEC/IEEE 20000-1 also proposes that the following should be quickly available following a major service failure or disaster to ensure continuity planning and testing: backups of data, documents and software, and any equipment or staff necessary for service restoration."</t>
   </si>
 </sst>
 </file>
@@ -1592,11 +1604,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L130"/>
+  <dimension ref="A1:L131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -3535,9 +3547,43 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G53" s="34"/>
-      <c r="J53" s="35"/>
+    <row r="53" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A53" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="15">
+        <v>52</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="I53" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="K53" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="L53" s="17" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="54" spans="1:12" ht="12.9" customHeight="1">
       <c r="G54" s="34"/>
@@ -3575,9 +3621,9 @@
       <c r="G62" s="34"/>
       <c r="J62" s="35"/>
     </row>
-    <row r="63" spans="1:12">
-      <c r="G63" s="20"/>
-      <c r="J63" s="32"/>
+    <row r="63" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G63" s="34"/>
+      <c r="J63" s="35"/>
     </row>
     <row r="64" spans="1:12">
       <c r="G64" s="20"/>
@@ -3847,13 +3893,17 @@
       <c r="G130" s="20"/>
       <c r="J130" s="32"/>
     </row>
+    <row r="131" spans="7:10">
+      <c r="G131" s="20"/>
+      <c r="J131" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D52" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D53" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F807" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F808" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -3908,12 +3958,13 @@
     <hyperlink ref="B48" r:id="rId47" xr:uid="{511DD410-6A69-43A8-8F3A-CAE2A8C507A0}"/>
     <hyperlink ref="B49" r:id="rId48" xr:uid="{F5B11D4C-86B2-48A4-96EC-35EA58FD9BD3}"/>
     <hyperlink ref="B50" r:id="rId49" xr:uid="{C2E5014C-5035-4F57-8116-A29BF9082082}"/>
-    <hyperlink ref="B52" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
+    <hyperlink ref="B53" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
     <hyperlink ref="B51" r:id="rId51" xr:uid="{BA099E17-6C3D-4BDD-8CDF-DABDDB357C20}"/>
+    <hyperlink ref="B52" r:id="rId52" xr:uid="{35ED0CE2-4BED-4515-BE35-B2CAFF31A346}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId52"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId53"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -3926,7 +3977,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G62</xm:sqref>
+          <xm:sqref>G2:G63</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add notes from rest of SWEBOK's maintenance chapter
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0955DB07-1FBF-4DBC-B5F1-050A6B4C330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CF0054-80FD-47B0-9D14-6F42E9D40802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="226">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -932,6 +932,74 @@
   </si>
   <si>
     <t>"ISO/IEC/IEEE 20000-1 also proposes that the following should be quickly available following a major service failure or disaster to ensure continuity planning and testing: backups of data, documents and software, and any equipment or staff necessary for service restoration."</t>
+  </si>
+  <si>
+    <t>4.4. Continuous Integration, Delivery, Testing and Deployment</t>
+  </si>
+  <si>
+    <t>Paras. 3-5</t>
+  </si>
+  <si>
+    <t>pp. 7-14 to 7-15</t>
+  </si>
+  <si>
+    <t>These paragraphs are VERY similar to paragraphs 2-4 of Section 6. Software Engineering Operations Tools of the Software Engineering Operations KA; one of these should be replaced to a pointer to the other to improve maintainability</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"For an explanation of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continuous delivery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continuous testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continuous deployment, see</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Section 6. Software Engineering Operations Tools of the Software Engineering Operations KA"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1604,11 +1672,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L131"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L53" sqref="L53"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -3585,9 +3653,43 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G54" s="34"/>
-      <c r="J54" s="35"/>
+    <row r="54" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A54" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="15">
+        <v>53</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I54" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="K54" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="L54" s="17" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="55" spans="1:12" ht="12.9" customHeight="1">
       <c r="G55" s="34"/>
@@ -3625,9 +3727,9 @@
       <c r="G63" s="34"/>
       <c r="J63" s="35"/>
     </row>
-    <row r="64" spans="1:12">
-      <c r="G64" s="20"/>
-      <c r="J64" s="32"/>
+    <row r="64" spans="1:12" ht="12.9" customHeight="1">
+      <c r="G64" s="34"/>
+      <c r="J64" s="35"/>
     </row>
     <row r="65" spans="7:10">
       <c r="G65" s="20"/>
@@ -3897,13 +3999,17 @@
       <c r="G131" s="20"/>
       <c r="J131" s="32"/>
     </row>
+    <row r="132" spans="7:10">
+      <c r="G132" s="20"/>
+      <c r="J132" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D53" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D54" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F808" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F809" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -3958,13 +4064,14 @@
     <hyperlink ref="B48" r:id="rId47" xr:uid="{511DD410-6A69-43A8-8F3A-CAE2A8C507A0}"/>
     <hyperlink ref="B49" r:id="rId48" xr:uid="{F5B11D4C-86B2-48A4-96EC-35EA58FD9BD3}"/>
     <hyperlink ref="B50" r:id="rId49" xr:uid="{C2E5014C-5035-4F57-8116-A29BF9082082}"/>
-    <hyperlink ref="B53" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
+    <hyperlink ref="B54" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
     <hyperlink ref="B51" r:id="rId51" xr:uid="{BA099E17-6C3D-4BDD-8CDF-DABDDB357C20}"/>
     <hyperlink ref="B52" r:id="rId52" xr:uid="{35ED0CE2-4BED-4515-BE35-B2CAFF31A346}"/>
+    <hyperlink ref="B53" r:id="rId53" xr:uid="{7BC7E498-C24F-4667-9B28-E50B03850850}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId53"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId54"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -3977,7 +4084,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G63</xm:sqref>
+          <xm:sqref>G2:G64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add more SWEBOK notes, up to but EXCLUDING 4. Software Quality Tools
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CF0054-80FD-47B0-9D14-6F42E9D40802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32787B3A-6141-4DA7-97B1-EFEEEB53A22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="244">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -598,9 +598,6 @@
   </si>
   <si>
     <t>"Fuzz testing" is the more common term used for what is called "fuzzy testing"; for example, ISO/IEC/IEEE 29119-1:2022 only uses the former</t>
-  </si>
-  <si>
-    <t>Should "Boundary-Value Analysis" and "All-Combinations Testing" have hyphens or no? They don't in ISO/IEC/IEEE 29119-4:2021, for example (see 3.3 and 3.12, respectively)</t>
   </si>
   <si>
     <t>Evidence-based testing isn't really defined/described, just how it applies to software engineering as a whole. What questions would be relevant? What kinds of evidence would be useful? It seems more like a "workflow" for designing other kinds of tests rather than an actual type of testing.</t>
@@ -1000,6 +997,63 @@
       </rPr>
       <t xml:space="preserve"> Section 6. Software Engineering Operations Tools of the Software Engineering Operations KA"</t>
     </r>
+  </si>
+  <si>
+    <t>3.4.2. Dynamic Analysis Techniques</t>
+  </si>
+  <si>
+    <t>Line 10</t>
+  </si>
+  <si>
+    <t>"In addition, black-box testing is …"</t>
+  </si>
+  <si>
+    <t>3.4.4. Software Quality Control and Testing</t>
+  </si>
+  <si>
+    <t>"Quality control is a set of activities that…"</t>
+  </si>
+  <si>
+    <t>Add hyphen to be consistent with the rest of the document and the literature</t>
+  </si>
+  <si>
+    <t>Use sentence case to be grammatically correct</t>
+  </si>
+  <si>
+    <t>3.4.5. Technical Reviews and Audits</t>
+  </si>
+  <si>
+    <t>Whole section</t>
+  </si>
+  <si>
+    <t>This section should be a subsection of 3.4.1. Static Analysis Techniques</t>
+  </si>
+  <si>
+    <t>Should "Boundary-Value Analysis" and "All-Combinations Testing" have hyphens or no? They don't in ISO/IEC/IEEE 29119-4:2021, for example (see 3.3 and 3.12, respectively); this change may want to be implemented for consistency with the literature</t>
+  </si>
+  <si>
+    <t>Reviews are a type of static analysis (peer reviews are given as an example of each)</t>
+  </si>
+  <si>
+    <t>pp. 12-13 to 12-14</t>
+  </si>
+  <si>
+    <t>Remove comma to be grammatically correct</t>
+  </si>
+  <si>
+    <t>"…(e.g., formal and informal)…"</t>
+  </si>
+  <si>
+    <t>Paras. 3 and 4</t>
+  </si>
+  <si>
+    <t>p. 12-14</t>
+  </si>
+  <si>
+    <t>Not only is the format of each review type presented in consistent (i.e., "…[review type] -- [definition]; …" vs. "…[review type] help ensure that [purpose]; …"), but it is also difficult to scan through them, see when one term starts and the next term ends, and compare/contrast the different types</t>
+  </si>
+  <si>
+    <t>Rewrite these lists of review types as bulleted lists</t>
   </si>
 </sst>
 </file>
@@ -1672,11 +1726,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1733,7 +1787,7 @@
     </row>
     <row r="2" spans="1:12" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>56</v>
@@ -1771,7 +1825,7 @@
     </row>
     <row r="3" spans="1:12" ht="56.5" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>56</v>
@@ -1803,7 +1857,7 @@
     </row>
     <row r="4" spans="1:12" ht="56.5" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>56</v>
@@ -1841,7 +1895,7 @@
     </row>
     <row r="5" spans="1:12" ht="56.5" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>56</v>
@@ -1879,7 +1933,7 @@
     </row>
     <row r="6" spans="1:12" ht="56.5" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>56</v>
@@ -1917,7 +1971,7 @@
     </row>
     <row r="7" spans="1:12" ht="56.5" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>56</v>
@@ -1955,7 +2009,7 @@
     </row>
     <row r="8" spans="1:12" ht="56.5" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>56</v>
@@ -1983,15 +2037,15 @@
         <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8" s="17" t="s">
         <v>197</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="56.5" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>56</v>
@@ -2024,12 +2078,12 @@
         <v>89</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="56.5" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>56</v>
@@ -2067,7 +2121,7 @@
     </row>
     <row r="11" spans="1:12" ht="56.5" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>56</v>
@@ -2100,12 +2154,12 @@
         <v>90</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="56.5" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>56</v>
@@ -2143,7 +2197,7 @@
     </row>
     <row r="13" spans="1:12" ht="56.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>56</v>
@@ -2176,12 +2230,12 @@
         <v>94</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="56.5" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>56</v>
@@ -2214,12 +2268,12 @@
         <v>95</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="56.5" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>56</v>
@@ -2250,12 +2304,12 @@
         <v>100</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="56.5" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>56</v>
@@ -2287,7 +2341,7 @@
     </row>
     <row r="17" spans="1:12" ht="56.5" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>56</v>
@@ -2325,7 +2379,7 @@
     </row>
     <row r="18" spans="1:12" ht="56.5" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>56</v>
@@ -2363,7 +2417,7 @@
     </row>
     <row r="19" spans="1:12" ht="56.5" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>56</v>
@@ -2401,7 +2455,7 @@
     </row>
     <row r="20" spans="1:12" ht="56.5" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>56</v>
@@ -2434,12 +2488,12 @@
         <v>116</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="56.5" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>56</v>
@@ -2472,12 +2526,12 @@
         <v>117</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="56.5" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>56</v>
@@ -2515,7 +2569,7 @@
     </row>
     <row r="23" spans="1:12" ht="56.5" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>56</v>
@@ -2553,7 +2607,7 @@
     </row>
     <row r="24" spans="1:12" ht="56.5" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>56</v>
@@ -2591,7 +2645,7 @@
     </row>
     <row r="25" spans="1:12" ht="56.5" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>56</v>
@@ -2615,15 +2669,15 @@
       <c r="I25" s="16"/>
       <c r="J25" s="31"/>
       <c r="K25" s="17" t="s">
-        <v>128</v>
+        <v>235</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="56.5" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>56</v>
@@ -2650,12 +2704,12 @@
         <v>127</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="56.5" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>56</v>
@@ -2676,22 +2730,22 @@
         <v>30</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="56.5" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>56</v>
@@ -2712,22 +2766,22 @@
         <v>30</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K28" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="L28" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="56.5" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>56</v>
@@ -2748,22 +2802,22 @@
         <v>30</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="56.5" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>56</v>
@@ -2784,22 +2838,22 @@
         <v>30</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="56.5" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>56</v>
@@ -2820,22 +2874,22 @@
         <v>30</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K31" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="L31" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="56.5" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>56</v>
@@ -2856,22 +2910,22 @@
         <v>30</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K32" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="L32" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="56.5" customHeight="1">
       <c r="A33" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>56</v>
@@ -2892,22 +2946,22 @@
         <v>30</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="56.5" customHeight="1">
       <c r="A34" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>56</v>
@@ -2928,22 +2982,22 @@
         <v>30</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="56.5" customHeight="1">
       <c r="A35" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>56</v>
@@ -2964,22 +3018,22 @@
         <v>30</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K35" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L35" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="56.5" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>56</v>
@@ -3000,24 +3054,24 @@
         <v>30</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J36" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K36" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="L36" s="17" t="s">
         <v>151</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="56.5" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>56</v>
@@ -3038,24 +3092,24 @@
         <v>30</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="J37" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="K37" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="L37" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="56.5" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>56</v>
@@ -3076,24 +3130,24 @@
         <v>30</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J38" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K38" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L38" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="56.5" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>56</v>
@@ -3114,24 +3168,24 @@
         <v>30</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I39" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="L39" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="J39" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="56.5" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>56</v>
@@ -3152,24 +3206,24 @@
         <v>30</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J40" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="K40" s="17" t="s">
-        <v>167</v>
-      </c>
       <c r="L40" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="56.5" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>56</v>
@@ -3190,24 +3244,24 @@
         <v>30</v>
       </c>
       <c r="H41" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J41" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="K41" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="J41" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="L41" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="56.25" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>56</v>
@@ -3228,24 +3282,24 @@
         <v>30</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K42" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L42" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="56.25" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>56</v>
@@ -3266,24 +3320,24 @@
         <v>30</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I43" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="56.25" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>56</v>
@@ -3304,24 +3358,24 @@
         <v>30</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I44" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J44" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="K44" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="L44" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="56.25" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>56</v>
@@ -3342,22 +3396,22 @@
         <v>30</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="K45" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="L45" s="17" t="s">
         <v>178</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="56.25" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" s="29" t="s">
         <v>56</v>
@@ -3378,22 +3432,22 @@
         <v>30</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K46" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="L46" s="17" t="s">
         <v>180</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="56.25" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>56</v>
@@ -3414,22 +3468,22 @@
         <v>30</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I47" s="16"/>
       <c r="J47" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K47" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="L47" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="L47" s="17" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="56.25" customHeight="1">
       <c r="A48" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B48" s="29" t="s">
         <v>56</v>
@@ -3450,22 +3504,22 @@
         <v>30</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I48" s="16"/>
       <c r="J48" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K48" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="L48" s="17" t="s">
         <v>185</v>
-      </c>
-      <c r="L48" s="17" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="56.25" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>56</v>
@@ -3486,24 +3540,24 @@
         <v>30</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I49" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J49" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K49" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="L49" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="L49" s="17" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="56.25" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>56</v>
@@ -3524,24 +3578,24 @@
         <v>30</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I50" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J50" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K50" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="L50" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="L50" s="17" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="56.25" customHeight="1">
       <c r="A51" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B51" s="29" t="s">
         <v>56</v>
@@ -3562,24 +3616,24 @@
         <v>30</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J51" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="L51" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="K51" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="L51" s="17" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="56.25" customHeight="1">
       <c r="A52" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B52" s="29" t="s">
         <v>56</v>
@@ -3600,24 +3654,24 @@
         <v>30</v>
       </c>
       <c r="H52" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="I52" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="I52" s="16" t="s">
+      <c r="J52" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="J52" s="31" t="s">
+      <c r="K52" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="L52" s="17" t="s">
         <v>215</v>
-      </c>
-      <c r="L52" s="17" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="56.25" customHeight="1">
       <c r="A53" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B53" s="29" t="s">
         <v>56</v>
@@ -3638,24 +3692,24 @@
         <v>31</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I53" s="16" t="s">
         <v>87</v>
       </c>
       <c r="J53" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="K53" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="L53" s="17" t="s">
         <v>219</v>
-      </c>
-      <c r="L53" s="17" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="56.25" customHeight="1">
       <c r="A54" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B54" s="29" t="s">
         <v>56</v>
@@ -3676,40 +3730,210 @@
         <v>32</v>
       </c>
       <c r="H54" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="I54" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I54" s="16" t="s">
+      <c r="J54" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="J54" s="31" t="s">
+      <c r="K54" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="K54" s="17" t="s">
+      <c r="L54" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="L54" s="17" t="s">
+    </row>
+    <row r="55" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A55" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" s="15">
+        <v>54</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" s="16" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G55" s="34"/>
-      <c r="J55" s="35"/>
-    </row>
-    <row r="56" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G56" s="34"/>
-      <c r="J56" s="35"/>
-    </row>
-    <row r="57" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G57" s="34"/>
-      <c r="J57" s="35"/>
-    </row>
-    <row r="58" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G58" s="34"/>
-      <c r="J58" s="35"/>
-    </row>
-    <row r="59" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G59" s="34"/>
-      <c r="J59" s="35"/>
+      <c r="I55" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J55" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="K55" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="L55" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A56" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" s="15">
+        <v>55</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="I56" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J56" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K56" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A57" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="15">
+        <v>56</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I57" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="J57" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A58" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="15">
+        <v>57</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H58" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I58" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J58" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="K58" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A59" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E59" s="15">
+        <v>58</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I59" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="J59" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="K59" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="12.9" customHeight="1">
       <c r="G60" s="34"/>
@@ -3731,25 +3955,25 @@
       <c r="G64" s="34"/>
       <c r="J64" s="35"/>
     </row>
-    <row r="65" spans="7:10">
-      <c r="G65" s="20"/>
-      <c r="J65" s="32"/>
-    </row>
-    <row r="66" spans="7:10">
-      <c r="G66" s="20"/>
-      <c r="J66" s="32"/>
-    </row>
-    <row r="67" spans="7:10">
-      <c r="G67" s="20"/>
-      <c r="J67" s="32"/>
-    </row>
-    <row r="68" spans="7:10">
-      <c r="G68" s="20"/>
-      <c r="J68" s="32"/>
-    </row>
-    <row r="69" spans="7:10">
-      <c r="G69" s="20"/>
-      <c r="J69" s="32"/>
+    <row r="65" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G65" s="34"/>
+      <c r="J65" s="35"/>
+    </row>
+    <row r="66" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G66" s="34"/>
+      <c r="J66" s="35"/>
+    </row>
+    <row r="67" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G67" s="34"/>
+      <c r="J67" s="35"/>
+    </row>
+    <row r="68" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G68" s="34"/>
+      <c r="J68" s="35"/>
+    </row>
+    <row r="69" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G69" s="34"/>
+      <c r="J69" s="35"/>
     </row>
     <row r="70" spans="7:10">
       <c r="G70" s="20"/>
@@ -4003,13 +4227,33 @@
       <c r="G132" s="20"/>
       <c r="J132" s="32"/>
     </row>
+    <row r="133" spans="7:10">
+      <c r="G133" s="20"/>
+      <c r="J133" s="32"/>
+    </row>
+    <row r="134" spans="7:10">
+      <c r="G134" s="20"/>
+      <c r="J134" s="32"/>
+    </row>
+    <row r="135" spans="7:10">
+      <c r="G135" s="20"/>
+      <c r="J135" s="32"/>
+    </row>
+    <row r="136" spans="7:10">
+      <c r="G136" s="20"/>
+      <c r="J136" s="32"/>
+    </row>
+    <row r="137" spans="7:10">
+      <c r="G137" s="20"/>
+      <c r="J137" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D54" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D59" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F809" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F814" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -4064,14 +4308,19 @@
     <hyperlink ref="B48" r:id="rId47" xr:uid="{511DD410-6A69-43A8-8F3A-CAE2A8C507A0}"/>
     <hyperlink ref="B49" r:id="rId48" xr:uid="{F5B11D4C-86B2-48A4-96EC-35EA58FD9BD3}"/>
     <hyperlink ref="B50" r:id="rId49" xr:uid="{C2E5014C-5035-4F57-8116-A29BF9082082}"/>
-    <hyperlink ref="B54" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
+    <hyperlink ref="B57" r:id="rId50" xr:uid="{3B20E4C5-25B3-4C68-91B2-4199B8E0E536}"/>
     <hyperlink ref="B51" r:id="rId51" xr:uid="{BA099E17-6C3D-4BDD-8CDF-DABDDB357C20}"/>
     <hyperlink ref="B52" r:id="rId52" xr:uid="{35ED0CE2-4BED-4515-BE35-B2CAFF31A346}"/>
     <hyperlink ref="B53" r:id="rId53" xr:uid="{7BC7E498-C24F-4667-9B28-E50B03850850}"/>
+    <hyperlink ref="B54" r:id="rId54" xr:uid="{A9F598D1-3995-43E2-9AD2-7CF13FCA7B71}"/>
+    <hyperlink ref="B55" r:id="rId55" xr:uid="{BF416F5B-CC32-48AB-B546-C94F4EA84815}"/>
+    <hyperlink ref="B56" r:id="rId56" xr:uid="{5E995981-9337-4957-A8DD-C5AB5922A4B4}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{CD3A2F53-33F6-40EC-87D8-BD75AB5F4CC3}"/>
+    <hyperlink ref="B58" r:id="rId58" xr:uid="{EEC18215-0FA0-471B-9FD7-E17204D62C3D}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId54"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId59"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -4084,7 +4333,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G64</xm:sqref>
+          <xm:sqref>G2:G69</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add notes from SWEBOK's Software Security chapter
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32787B3A-6141-4DA7-97B1-EFEEEB53A22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF4D2C-3BC3-445F-91FC-3D4D180C44D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="254">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -1054,6 +1054,66 @@
   </si>
   <si>
     <t>Rewrite these lists of review types as bulleted lists</t>
+  </si>
+  <si>
+    <t>4.5. Security Testing</t>
+  </si>
+  <si>
+    <t>pp. 13-4 to 13-5</t>
+  </si>
+  <si>
+    <t>The definition of "penetration testing" should appear where the term is first used</t>
+  </si>
+  <si>
+    <t>Move the definition of penetration testing in 5.2. Penetration Testing Tools to this section</t>
+  </si>
+  <si>
+    <t>5.2. Penetration Testing Tools</t>
+  </si>
+  <si>
+    <t>p. 13-5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No information is given here that is actually about the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">tools </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>for this testing, just about the testing itself; after No. 59, there will be no meaningful content in this section</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Either remove this section or add information specific about penetration testing </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tools</t>
+    </r>
+  </si>
+  <si>
+    <t>6.3. Security for Machine Learning-Based Application</t>
+  </si>
+  <si>
+    <t>"…presents a specific vulnerability: attackers…"</t>
   </si>
 </sst>
 </file>
@@ -1726,11 +1786,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L137"/>
+  <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -3935,17 +3995,119 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G60" s="34"/>
-      <c r="J60" s="35"/>
-    </row>
-    <row r="61" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G61" s="34"/>
-      <c r="J61" s="35"/>
-    </row>
-    <row r="62" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G62" s="34"/>
-      <c r="J62" s="35"/>
+    <row r="60" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A60" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" s="15">
+        <v>59</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I60" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="J60" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="K60" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A61" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61" s="15">
+        <v>60</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="I61" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="J61" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A62" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E62" s="15">
+        <v>61</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J62" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="K62" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="L62" s="17" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="63" spans="1:12" ht="12.9" customHeight="1">
       <c r="G63" s="34"/>
@@ -3975,17 +4137,17 @@
       <c r="G69" s="34"/>
       <c r="J69" s="35"/>
     </row>
-    <row r="70" spans="7:10">
-      <c r="G70" s="20"/>
-      <c r="J70" s="32"/>
-    </row>
-    <row r="71" spans="7:10">
-      <c r="G71" s="20"/>
-      <c r="J71" s="32"/>
-    </row>
-    <row r="72" spans="7:10">
-      <c r="G72" s="20"/>
-      <c r="J72" s="32"/>
+    <row r="70" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G70" s="34"/>
+      <c r="J70" s="35"/>
+    </row>
+    <row r="71" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G71" s="34"/>
+      <c r="J71" s="35"/>
+    </row>
+    <row r="72" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G72" s="34"/>
+      <c r="J72" s="35"/>
     </row>
     <row r="73" spans="7:10">
       <c r="G73" s="20"/>
@@ -4247,13 +4409,25 @@
       <c r="G137" s="20"/>
       <c r="J137" s="32"/>
     </row>
+    <row r="138" spans="7:10">
+      <c r="G138" s="20"/>
+      <c r="J138" s="32"/>
+    </row>
+    <row r="139" spans="7:10">
+      <c r="G139" s="20"/>
+      <c r="J139" s="32"/>
+    </row>
+    <row r="140" spans="7:10">
+      <c r="G140" s="20"/>
+      <c r="J140" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D59" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D62" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F814" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F817" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -4317,10 +4491,13 @@
     <hyperlink ref="B56" r:id="rId56" xr:uid="{5E995981-9337-4957-A8DD-C5AB5922A4B4}"/>
     <hyperlink ref="B59" r:id="rId57" xr:uid="{CD3A2F53-33F6-40EC-87D8-BD75AB5F4CC3}"/>
     <hyperlink ref="B58" r:id="rId58" xr:uid="{EEC18215-0FA0-471B-9FD7-E17204D62C3D}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{2DB19159-1DC5-4266-9B69-1081908455EE}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{3637FD25-33B5-483E-BFE3-D0778E83EF06}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{D42ADDB5-2F62-434D-AD8B-01412A072510}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId59"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId62"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -4333,7 +4510,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G69</xm:sqref>
+          <xm:sqref>G2:G72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add rest of notes and feedback on SWEBOK v4
Hopefully we're done now! :sweat_smile:
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF4D2C-3BC3-445F-91FC-3D4D180C44D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE53AF6-9BA0-41AE-B1AB-AD44332C7275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="259">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -1114,6 +1114,21 @@
   </si>
   <si>
     <t>"…presents a specific vulnerability: attackers…"</t>
+  </si>
+  <si>
+    <t>Whole document</t>
+  </si>
+  <si>
+    <t>Text formatted as code doesn't display nicely when one variable name is justified (the letters get spread across the line)</t>
+  </si>
+  <si>
+    <t>Reformat lines of code with only a single variable to not be justified</t>
+  </si>
+  <si>
+    <t>Code is usually displayed with a monospace font; doing this improves readability and consistency with other documentation</t>
+  </si>
+  <si>
+    <t>Reformat lines of code to use a monospace font</t>
   </si>
 </sst>
 </file>
@@ -1786,11 +1801,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L140"/>
+  <dimension ref="A1:L142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I66" sqref="I66"/>
+      <selection pane="bottomLeft" activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -4109,13 +4124,73 @@
         <v>253</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G63" s="34"/>
-      <c r="J63" s="35"/>
-    </row>
-    <row r="64" spans="1:12" ht="12.9" customHeight="1">
-      <c r="G64" s="34"/>
-      <c r="J64" s="35"/>
+    <row r="63" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A63" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E63" s="15">
+        <v>62</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="I63" s="16"/>
+      <c r="J63" s="31"/>
+      <c r="K63" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="L63" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="56.25" customHeight="1">
+      <c r="A64" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="15">
+        <v>63</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="I64" s="16"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="L64" s="17" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="65" spans="7:10" ht="12.9" customHeight="1">
       <c r="G65" s="34"/>
@@ -4149,13 +4224,13 @@
       <c r="G72" s="34"/>
       <c r="J72" s="35"/>
     </row>
-    <row r="73" spans="7:10">
-      <c r="G73" s="20"/>
-      <c r="J73" s="32"/>
-    </row>
-    <row r="74" spans="7:10">
-      <c r="G74" s="20"/>
-      <c r="J74" s="32"/>
+    <row r="73" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G73" s="34"/>
+      <c r="J73" s="35"/>
+    </row>
+    <row r="74" spans="7:10" ht="12.9" customHeight="1">
+      <c r="G74" s="34"/>
+      <c r="J74" s="35"/>
     </row>
     <row r="75" spans="7:10">
       <c r="G75" s="20"/>
@@ -4421,13 +4496,21 @@
       <c r="G140" s="20"/>
       <c r="J140" s="32"/>
     </row>
+    <row r="141" spans="7:10">
+      <c r="G141" s="20"/>
+      <c r="J141" s="32"/>
+    </row>
+    <row r="142" spans="7:10">
+      <c r="G142" s="20"/>
+      <c r="J142" s="32"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D62" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D64" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F817" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F819" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Category</formula1>
     </dataValidation>
   </dataValidations>
@@ -4494,10 +4577,12 @@
     <hyperlink ref="B60" r:id="rId59" xr:uid="{2DB19159-1DC5-4266-9B69-1081908455EE}"/>
     <hyperlink ref="B61" r:id="rId60" xr:uid="{3637FD25-33B5-483E-BFE3-D0778E83EF06}"/>
     <hyperlink ref="B62" r:id="rId61" xr:uid="{D42ADDB5-2F62-434D-AD8B-01412A072510}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{0D4CE8DE-1685-4480-82B4-DCB70E3E57C2}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{99DD474B-C3D4-4A84-8DF2-DBB35B169278}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.74803149606299213" top="0.78740157480314965" bottom="0.70866141732283472" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId62"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="1100" orientation="landscape" r:id="rId64"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Arial,Bold"Commenting template (Version 5)&amp;R&amp;"Arial,Bold"ISO/IEC JTC 1/SC 7/WG 7 N0808
 2004-09-05</oddHeader>
@@ -4510,7 +4595,7 @@
           <x14:formula1>
             <xm:f>'(list)'!$A$1:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G72</xm:sqref>
+          <xm:sqref>G2:G74</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fix category of general edits in my feedback
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE53AF6-9BA0-41AE-B1AB-AD44332C7275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4EDBE8-5498-466A-A7F1-4E3E29786DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1805,7 +1805,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L64" sqref="L64"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -4141,7 +4141,7 @@
         <v>62</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G63" s="19" t="s">
         <v>43</v>
@@ -4175,7 +4175,7 @@
         <v>63</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G64" s="19" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Investigate which suggestions I made were accepted by SWEBOK; #241
Append analysis to original review submission
Create pie charts summarizing how these suggestions were handled
</commit_message>
<xml_diff>
--- a/SWEBOK4-SamuelCrawford.xlsx
+++ b/SWEBOK4-SamuelCrawford.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestGen-Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\TestingTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4EDBE8-5498-466A-A7F1-4E3E29786DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A13A3D-B94C-403A-A190-063FF00F12B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comments!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comments!$M$1:$M$142</definedName>
     <definedName name="Category">Categories!$B$4:$B$8</definedName>
     <definedName name="ccc">[1]Categories!$B$4:$B$8</definedName>
     <definedName name="OLE_LINK5" localSheetId="0">Comments!#REF!</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="287">
   <si>
     <r>
       <t xml:space="preserve">Covers grammar, missing or duplicated text, missing or incorrect cross-references, incorrect numbering, spelling and punctuation problems. These are all matters that should be able to be resolved offline by the Project Editor.  Terminology changes are not Editorial e.g. Enterprise versus Organization.  
@@ -1129,6 +1129,116 @@
   </si>
   <si>
     <t>Reformat lines of code to use a monospace font</t>
+  </si>
+  <si>
+    <t>Addressed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Partially</t>
+  </si>
+  <si>
+    <t>Incorrectly</t>
+  </si>
+  <si>
+    <t>"…is not always possible, additional business domain expertise might be necessary.…"</t>
+  </si>
+  <si>
+    <t>Modified Text/Notes</t>
+  </si>
+  <si>
+    <t>May have been ignored for brevity</t>
+  </si>
+  <si>
+    <t>"Managing (i.e., identifying, solving or removing) the infeasible paths…"</t>
+  </si>
+  <si>
+    <t>"…and code annotations. The automation of oracles can be…"</t>
+  </si>
+  <si>
+    <t>"…Additionally, the detection of infeasible paths can also play a role in reducing security vulnerabilities.…"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"…formerly documented as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SWEBOK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2004; this…"
+May have been ignored for traceability/consistency</t>
+    </r>
+  </si>
+  <si>
+    <t>May have been ignored for traceability/consistency</t>
+  </si>
+  <si>
+    <t>"…are important evidences for software testing…"
+Is this grammatically/conceptually correct?</t>
+  </si>
+  <si>
+    <t>"Scalability testing assesses the software’s ability to scale up non-functional requirements such as load, number of transactions, volume of data. It could integrate or extend load, elasticity and stress testing."
+No definition provided for "usability testing", despite including it in the introduction</t>
+  </si>
+  <si>
+    <t>"…whether the components’ interface provide the correct…"</t>
+  </si>
+  <si>
+    <t>"Boundary-Value Analysis" still appears in Table of Contents</t>
+  </si>
+  <si>
+    <t>The statement that "these principles can also be applied to the testing process" was moved to a bullet point, which makes the issue I had less noticable without addressing it!</t>
+  </si>
+  <si>
+    <t>Was this even necessary?</t>
+  </si>
+  <si>
+    <t>"Monkey testing runs randomly generated test cases to simulate rundom activities and cause the program to stop."
+Note the typo of "rundom"</t>
+  </si>
+  <si>
+    <t>"Buddy testing" was given as a synonym of "pair testing", and its relevant information omitted</t>
+  </si>
+  <si>
+    <t>"Quick testing, in which a very small test suite is selected and executed to swiftly identify critical issues in the SUT. It aims to enhances the probability of detecting faults early in the development process."
+This definition is full of grammatical errors</t>
+  </si>
+  <si>
+    <t>May have been ignored intentionally</t>
+  </si>
+  <si>
+    <t>Defined in Sec. 3.1 Operational Testing, Verification, and Acceptance, which maybe makes this obsolete</t>
+  </si>
+  <si>
+    <t>The caveat of "nowadays" is added that doesn't address this concern</t>
+  </si>
+  <si>
+    <t>A missing space that I missed---"…installation of software.[1, s6.4.13.3 Note 1].…"---is still present, and it is unnecessary to include brackets when adapting the capitalization of quoted text, such as in "…pointed out that '[t]he biggest risk…"</t>
+  </si>
+  <si>
+    <t>The list of reviews in Para. 3 was made into a bulleted list, but not the one in Para. 4.</t>
+  </si>
+  <si>
+    <t>"…presents a specific vulnerability. Attackers…"
+Doesn't flow as well, but is grammatically correct</t>
+  </si>
+  <si>
+    <t>"Elasticity testing assesses the ability of the SUT (such as cloud and distributed systems) to rapidly expand or shrink compute, memory, and storage resources without compromising the capacity to meet peak utilization. Some elasticity testing objectives are to control behaviors, to identify the resources to be (un)allocated, and to coordinate events in parallel."
+Source supports the second sentence, but not explicitly the first</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1373,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1374,6 +1484,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1389,7 +1505,162 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_WG 71" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1801,11 +2072,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L142"/>
+  <dimension ref="A1:N142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.9"/>
@@ -1820,9 +2091,11 @@
     <col min="9" max="9" width="10.81640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="8.08984375" style="33" customWidth="1"/>
     <col min="11" max="12" width="47.7265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="2"/>
+    <col min="14" max="14" width="47.7265625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.549999999999997" customHeight="1">
+    <row r="1" spans="1:14" ht="39.549999999999997" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>54</v>
       </c>
@@ -1859,8 +2132,14 @@
       <c r="L1" s="25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M1" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="56.5" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>190</v>
       </c>
@@ -1897,8 +2176,14 @@
       <c r="L2" s="17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="56.5" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>190</v>
       </c>
@@ -1929,8 +2214,12 @@
       <c r="L3" s="17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M3" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N3" s="36"/>
+    </row>
+    <row r="4" spans="1:14" ht="56.5" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>190</v>
       </c>
@@ -1967,8 +2256,14 @@
       <c r="L4" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M4" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N4" s="36" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="56.5" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>190</v>
       </c>
@@ -2005,8 +2300,14 @@
       <c r="L5" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M5" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="56.5" customHeight="1">
       <c r="A6" s="18" t="s">
         <v>190</v>
       </c>
@@ -2043,8 +2344,14 @@
       <c r="L6" s="17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M6" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="56.5" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>190</v>
       </c>
@@ -2081,8 +2388,12 @@
       <c r="L7" s="17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M7" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="1:14" ht="56.5" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>190</v>
       </c>
@@ -2117,8 +2428,12 @@
       <c r="L8" s="17" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M8" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N8" s="36"/>
+    </row>
+    <row r="9" spans="1:14" ht="56.5" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>190</v>
       </c>
@@ -2155,8 +2470,14 @@
       <c r="L9" s="17" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M9" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N9" s="36" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="56.5" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>190</v>
       </c>
@@ -2193,8 +2514,14 @@
       <c r="L10" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="56.5" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>190</v>
       </c>
@@ -2231,8 +2558,14 @@
       <c r="L11" s="17" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="56.5" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>190</v>
       </c>
@@ -2269,8 +2602,14 @@
       <c r="L12" s="17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M12" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="56.5" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>190</v>
       </c>
@@ -2307,8 +2646,14 @@
       <c r="L13" s="17" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="56.5" customHeight="1">
       <c r="A14" s="18" t="s">
         <v>190</v>
       </c>
@@ -2345,8 +2690,14 @@
       <c r="L14" s="17" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M14" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="56.5" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>190</v>
       </c>
@@ -2381,8 +2732,12 @@
       <c r="L15" s="17" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M15" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N15" s="36"/>
+    </row>
+    <row r="16" spans="1:14" ht="56.5" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>190</v>
       </c>
@@ -2413,8 +2768,12 @@
       <c r="L16" s="17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M16" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N16" s="36"/>
+    </row>
+    <row r="17" spans="1:14" ht="56.5" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>190</v>
       </c>
@@ -2451,8 +2810,12 @@
       <c r="L17" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M17" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N17" s="36"/>
+    </row>
+    <row r="18" spans="1:14" ht="56.5" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>190</v>
       </c>
@@ -2489,8 +2852,12 @@
       <c r="L18" s="17" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M18" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="36"/>
+    </row>
+    <row r="19" spans="1:14" ht="56.5" customHeight="1">
       <c r="A19" s="18" t="s">
         <v>190</v>
       </c>
@@ -2527,8 +2894,12 @@
       <c r="L19" s="17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M19" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" s="36"/>
+    </row>
+    <row r="20" spans="1:14" ht="56.5" customHeight="1">
       <c r="A20" s="18" t="s">
         <v>190</v>
       </c>
@@ -2565,8 +2936,14 @@
       <c r="L20" s="17" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M20" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N20" s="36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="56.5" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>190</v>
       </c>
@@ -2603,8 +2980,14 @@
       <c r="L21" s="17" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M21" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N21" s="36" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="56.5" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>190</v>
       </c>
@@ -2641,8 +3024,12 @@
       <c r="L22" s="17" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M22" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="36"/>
+    </row>
+    <row r="23" spans="1:14" ht="56.5" customHeight="1">
       <c r="A23" s="18" t="s">
         <v>190</v>
       </c>
@@ -2679,8 +3066,12 @@
       <c r="L23" s="17" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="36"/>
+    </row>
+    <row r="24" spans="1:14" ht="56.5" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>190</v>
       </c>
@@ -2717,8 +3108,14 @@
       <c r="L24" s="17" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M24" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N24" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="56.5" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>190</v>
       </c>
@@ -2749,8 +3146,14 @@
       <c r="L25" s="17" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M25" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N25" s="36" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="56.5" customHeight="1">
       <c r="A26" s="18" t="s">
         <v>190</v>
       </c>
@@ -2781,8 +3184,12 @@
       <c r="L26" s="17" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="36"/>
+    </row>
+    <row r="27" spans="1:14" ht="56.5" customHeight="1">
       <c r="A27" s="18" t="s">
         <v>190</v>
       </c>
@@ -2817,8 +3224,14 @@
       <c r="L27" s="17" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M27" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N27" s="36" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="56.5" customHeight="1">
       <c r="A28" s="18" t="s">
         <v>190</v>
       </c>
@@ -2853,8 +3266,14 @@
       <c r="L28" s="17" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M28" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N28" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="56.5" customHeight="1">
       <c r="A29" s="18" t="s">
         <v>190</v>
       </c>
@@ -2889,8 +3308,12 @@
       <c r="L29" s="17" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M29" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N29" s="36"/>
+    </row>
+    <row r="30" spans="1:14" ht="56.5" customHeight="1">
       <c r="A30" s="18" t="s">
         <v>190</v>
       </c>
@@ -2925,8 +3348,12 @@
       <c r="L30" s="17" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M30" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N30" s="36"/>
+    </row>
+    <row r="31" spans="1:14" ht="56.5" customHeight="1">
       <c r="A31" s="18" t="s">
         <v>190</v>
       </c>
@@ -2961,8 +3388,14 @@
       <c r="L31" s="17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M31" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N31" s="36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="56.5" customHeight="1">
       <c r="A32" s="18" t="s">
         <v>190</v>
       </c>
@@ -2997,8 +3430,12 @@
       <c r="L32" s="17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M32" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N32" s="36"/>
+    </row>
+    <row r="33" spans="1:14" ht="56.5" customHeight="1">
       <c r="A33" s="18" t="s">
         <v>190</v>
       </c>
@@ -3033,8 +3470,12 @@
       <c r="L33" s="17" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M33" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N33" s="36"/>
+    </row>
+    <row r="34" spans="1:14" ht="56.5" customHeight="1">
       <c r="A34" s="18" t="s">
         <v>190</v>
       </c>
@@ -3069,8 +3510,12 @@
       <c r="L34" s="17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M34" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N34" s="36"/>
+    </row>
+    <row r="35" spans="1:14" ht="56.5" customHeight="1">
       <c r="A35" s="18" t="s">
         <v>190</v>
       </c>
@@ -3105,8 +3550,12 @@
       <c r="L35" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M35" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N35" s="36"/>
+    </row>
+    <row r="36" spans="1:14" ht="56.5" customHeight="1">
       <c r="A36" s="18" t="s">
         <v>190</v>
       </c>
@@ -3143,8 +3592,12 @@
       <c r="L36" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M36" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N36" s="36"/>
+    </row>
+    <row r="37" spans="1:14" ht="56.5" customHeight="1">
       <c r="A37" s="18" t="s">
         <v>190</v>
       </c>
@@ -3181,8 +3634,14 @@
       <c r="L37" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M37" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N37" s="36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="56.5" customHeight="1">
       <c r="A38" s="18" t="s">
         <v>190</v>
       </c>
@@ -3219,8 +3678,14 @@
       <c r="L38" s="17" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M38" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N38" s="36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="56.5" customHeight="1">
       <c r="A39" s="18" t="s">
         <v>190</v>
       </c>
@@ -3257,8 +3722,12 @@
       <c r="L39" s="17" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M39" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N39" s="36"/>
+    </row>
+    <row r="40" spans="1:14" ht="56.5" customHeight="1">
       <c r="A40" s="18" t="s">
         <v>190</v>
       </c>
@@ -3295,8 +3764,12 @@
       <c r="L40" s="17" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="56.5" customHeight="1">
+      <c r="M40" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N40" s="36"/>
+    </row>
+    <row r="41" spans="1:14" ht="56.5" customHeight="1">
       <c r="A41" s="18" t="s">
         <v>190</v>
       </c>
@@ -3333,8 +3806,14 @@
       <c r="L41" s="17" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M41" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N41" s="36" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="56.25" customHeight="1">
       <c r="A42" s="18" t="s">
         <v>190</v>
       </c>
@@ -3371,8 +3850,12 @@
       <c r="L42" s="17" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M42" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N42" s="36"/>
+    </row>
+    <row r="43" spans="1:14" ht="56.25" customHeight="1">
       <c r="A43" s="18" t="s">
         <v>190</v>
       </c>
@@ -3409,8 +3892,12 @@
       <c r="L43" s="17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M43" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N43" s="36"/>
+    </row>
+    <row r="44" spans="1:14" ht="56.25" customHeight="1">
       <c r="A44" s="18" t="s">
         <v>190</v>
       </c>
@@ -3447,8 +3934,14 @@
       <c r="L44" s="17" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M44" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N44" s="36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="56.25" customHeight="1">
       <c r="A45" s="18" t="s">
         <v>190</v>
       </c>
@@ -3483,8 +3976,14 @@
       <c r="L45" s="17" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M45" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N45" s="36" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="56.25" customHeight="1">
       <c r="A46" s="18" t="s">
         <v>190</v>
       </c>
@@ -3519,8 +4018,14 @@
       <c r="L46" s="17" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M46" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="N46" s="36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="56.25" customHeight="1">
       <c r="A47" s="18" t="s">
         <v>190</v>
       </c>
@@ -3555,8 +4060,12 @@
       <c r="L47" s="17" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M47" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N47" s="36"/>
+    </row>
+    <row r="48" spans="1:14" ht="56.25" customHeight="1">
       <c r="A48" s="18" t="s">
         <v>190</v>
       </c>
@@ -3591,8 +4100,12 @@
       <c r="L48" s="17" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M48" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N48" s="36"/>
+    </row>
+    <row r="49" spans="1:14" ht="56.25" customHeight="1">
       <c r="A49" s="18" t="s">
         <v>190</v>
       </c>
@@ -3629,8 +4142,12 @@
       <c r="L49" s="17" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M49" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N49" s="36"/>
+    </row>
+    <row r="50" spans="1:14" ht="56.25" customHeight="1">
       <c r="A50" s="18" t="s">
         <v>190</v>
       </c>
@@ -3667,8 +4184,12 @@
       <c r="L50" s="17" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M50" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N50" s="36"/>
+    </row>
+    <row r="51" spans="1:14" ht="56.25" customHeight="1">
       <c r="A51" s="18" t="s">
         <v>190</v>
       </c>
@@ -3705,8 +4226,12 @@
       <c r="L51" s="17" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M51" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N51" s="36"/>
+    </row>
+    <row r="52" spans="1:14" ht="56.25" customHeight="1">
       <c r="A52" s="18" t="s">
         <v>190</v>
       </c>
@@ -3743,8 +4268,12 @@
       <c r="L52" s="17" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M52" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N52" s="36"/>
+    </row>
+    <row r="53" spans="1:14" ht="56.25" customHeight="1">
       <c r="A53" s="18" t="s">
         <v>190</v>
       </c>
@@ -3781,8 +4310,12 @@
       <c r="L53" s="17" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M53" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N53" s="36"/>
+    </row>
+    <row r="54" spans="1:14" ht="56.25" customHeight="1">
       <c r="A54" s="18" t="s">
         <v>190</v>
       </c>
@@ -3819,8 +4352,14 @@
       <c r="L54" s="17" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M54" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N54" s="36" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="56.25" customHeight="1">
       <c r="A55" s="18" t="s">
         <v>190</v>
       </c>
@@ -3857,8 +4396,12 @@
       <c r="L55" s="17" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M55" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N55" s="36"/>
+    </row>
+    <row r="56" spans="1:14" ht="56.25" customHeight="1">
       <c r="A56" s="18" t="s">
         <v>190</v>
       </c>
@@ -3895,8 +4438,14 @@
       <c r="L56" s="17" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M56" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N56" s="36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="56.25" customHeight="1">
       <c r="A57" s="18" t="s">
         <v>190</v>
       </c>
@@ -3933,8 +4482,12 @@
       <c r="L57" s="17" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M57" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N57" s="36"/>
+    </row>
+    <row r="58" spans="1:14" ht="56.25" customHeight="1">
       <c r="A58" s="18" t="s">
         <v>190</v>
       </c>
@@ -3971,8 +4524,12 @@
       <c r="L58" s="17" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M58" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="N58" s="36"/>
+    </row>
+    <row r="59" spans="1:14" ht="56.25" customHeight="1">
       <c r="A59" s="18" t="s">
         <v>190</v>
       </c>
@@ -4009,8 +4566,14 @@
       <c r="L59" s="17" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M59" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="N59" s="36" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="56.25" customHeight="1">
       <c r="A60" s="18" t="s">
         <v>190</v>
       </c>
@@ -4047,8 +4610,12 @@
       <c r="L60" s="17" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M60" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N60" s="36"/>
+    </row>
+    <row r="61" spans="1:14" ht="56.25" customHeight="1">
       <c r="A61" s="18" t="s">
         <v>190</v>
       </c>
@@ -4085,8 +4652,12 @@
       <c r="L61" s="17" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M61" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N61" s="36"/>
+    </row>
+    <row r="62" spans="1:14" ht="56.25" customHeight="1">
       <c r="A62" s="18" t="s">
         <v>190</v>
       </c>
@@ -4123,8 +4694,14 @@
       <c r="L62" s="17" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M62" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="56.25" customHeight="1">
       <c r="A63" s="18" t="s">
         <v>190</v>
       </c>
@@ -4157,8 +4734,12 @@
       <c r="L63" s="17" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="56.25" customHeight="1">
+      <c r="M63" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N63" s="36"/>
+    </row>
+    <row r="64" spans="1:14" ht="56.25" customHeight="1">
       <c r="A64" s="18" t="s">
         <v>190</v>
       </c>
@@ -4191,6 +4772,10 @@
       <c r="L64" s="17" t="s">
         <v>258</v>
       </c>
+      <c r="M64" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N64" s="36"/>
     </row>
     <row r="65" spans="7:10" ht="12.9" customHeight="1">
       <c r="G65" s="34"/>
@@ -4505,7 +5090,30 @@
       <c r="J142" s="32"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N64">
+    <sortCondition ref="E1:E64"/>
+  </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Incorrectly">
+      <formula>NOT(ISERROR(SEARCH("Incorrectly",M1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Incompletely">
+      <formula>NOT(ISERROR(SEARCH("Incompletely",M1)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="7" priority="7" operator="notContains" text="Addressed">
+      <formula>ISERROR(SEARCH("Addressed",M1))</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="6" priority="5" stopIfTrue="1">
+      <formula>LEN(TRIM(M1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D64" xr:uid="{D665B289-B899-4E8C-BCED-2245F91E51F7}">
       <formula1>"Yes,No"</formula1>
@@ -4698,11 +5306,11 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="42.75" customHeight="1">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="9" t="s">
@@ -4710,11 +5318,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="35.25" customHeight="1">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="9" t="s">
@@ -4722,11 +5330,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="57" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
@@ -4734,11 +5342,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="47.25" customHeight="1">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
@@ -4746,11 +5354,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="57.75" customHeight="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>